<commit_message>
Add TIMSS 2019 G4 student questionnaire cleaning
</commit_message>
<xml_diff>
--- a/2_TIMSS_2019_G4_clean/Instructions.xlsx
+++ b/2_TIMSS_2019_G4_clean/Instructions.xlsx
@@ -5,36 +5,36 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\data\TIMSS_2019_G4_clean\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\TIMSS_2019\2_TIMSS_2019_G4_clean\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94E15513-E5CC-4CA9-8DA0-D9A085C4ED0A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9866A97C-1D25-42C9-87FB-BD87012FCBD1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" tabRatio="730" xr2:uid="{6A18A5C5-ACE7-445C-877F-08C8BDB6A624}"/>
+    <workbookView xWindow="-23148" yWindow="4284" windowWidth="23256" windowHeight="12576" tabRatio="730" activeTab="2" xr2:uid="{6A18A5C5-ACE7-445C-877F-08C8BDB6A624}"/>
   </bookViews>
   <sheets>
-    <sheet name="0_G4_PV" sheetId="14" r:id="rId1"/>
-    <sheet name="1_G4_Teacher" sheetId="15" r:id="rId2"/>
-    <sheet name="2_G4_Student" sheetId="16" r:id="rId3"/>
-    <sheet name="3_G4_Parent" sheetId="17" r:id="rId4"/>
-    <sheet name="4_G4_School" sheetId="18" r:id="rId5"/>
-    <sheet name="0_G8_PV" sheetId="19" r:id="rId6"/>
-    <sheet name="1_G8_Teacher_M" sheetId="20" r:id="rId7"/>
-    <sheet name="2_G8_Teacher_S" sheetId="21" r:id="rId8"/>
-    <sheet name="3_G8_Student" sheetId="22" r:id="rId9"/>
-    <sheet name="4_G8_School" sheetId="23" r:id="rId10"/>
+    <sheet name="1_G4_PV" sheetId="14" r:id="rId1"/>
+    <sheet name="2_G4_Teacher" sheetId="15" r:id="rId2"/>
+    <sheet name="3_G4_Student" sheetId="16" r:id="rId3"/>
+    <sheet name="4_G4_Parent" sheetId="17" r:id="rId4"/>
+    <sheet name="5_G4_School" sheetId="18" r:id="rId5"/>
+    <sheet name="6_G8_PV" sheetId="19" r:id="rId6"/>
+    <sheet name="7_G8_Teacher_M" sheetId="20" r:id="rId7"/>
+    <sheet name="8_G8_Teacher_S" sheetId="21" r:id="rId8"/>
+    <sheet name="9_G8_Student" sheetId="22" r:id="rId9"/>
+    <sheet name="10_G8_School" sheetId="23" r:id="rId10"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Titles" localSheetId="0">'0_G4_PV'!$1:$1</definedName>
-    <definedName name="_xlnm.Print_Titles" localSheetId="5">'0_G8_PV'!$1:$1</definedName>
-    <definedName name="_xlnm.Print_Titles" localSheetId="1">'1_G4_Teacher'!$1:$1</definedName>
-    <definedName name="_xlnm.Print_Titles" localSheetId="6">'1_G8_Teacher_M'!$1:$1</definedName>
-    <definedName name="_xlnm.Print_Titles" localSheetId="2">'2_G4_Student'!$1:$1</definedName>
-    <definedName name="_xlnm.Print_Titles" localSheetId="7">'2_G8_Teacher_S'!$1:$1</definedName>
-    <definedName name="_xlnm.Print_Titles" localSheetId="3">'3_G4_Parent'!$1:$1</definedName>
-    <definedName name="_xlnm.Print_Titles" localSheetId="8">'3_G8_Student'!$1:$1</definedName>
-    <definedName name="_xlnm.Print_Titles" localSheetId="4">'4_G4_School'!$1:$1</definedName>
-    <definedName name="_xlnm.Print_Titles" localSheetId="9">'4_G8_School'!$1:$1</definedName>
+    <definedName name="_xlnm.Print_Titles" localSheetId="0">'1_G4_PV'!$1:$1</definedName>
+    <definedName name="_xlnm.Print_Titles" localSheetId="9">'10_G8_School'!$1:$1</definedName>
+    <definedName name="_xlnm.Print_Titles" localSheetId="1">'2_G4_Teacher'!$1:$1</definedName>
+    <definedName name="_xlnm.Print_Titles" localSheetId="2">'3_G4_Student'!$1:$1</definedName>
+    <definedName name="_xlnm.Print_Titles" localSheetId="3">'4_G4_Parent'!$1:$1</definedName>
+    <definedName name="_xlnm.Print_Titles" localSheetId="4">'5_G4_School'!$1:$1</definedName>
+    <definedName name="_xlnm.Print_Titles" localSheetId="5">'6_G8_PV'!$1:$1</definedName>
+    <definedName name="_xlnm.Print_Titles" localSheetId="6">'7_G8_Teacher_M'!$1:$1</definedName>
+    <definedName name="_xlnm.Print_Titles" localSheetId="7">'8_G8_Teacher_S'!$1:$1</definedName>
+    <definedName name="_xlnm.Print_Titles" localSheetId="8">'9_G8_Student'!$1:$1</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -11417,7 +11417,7 @@
   </sheetPr>
   <dimension ref="A1:G106"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft"/>
     </sheetView>
@@ -13105,7 +13105,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft"/>
+      <selection pane="bottomLeft" activeCell="E33" sqref="E33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -20226,7 +20226,7 @@
   </sheetPr>
   <dimension ref="A1:G145"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft"/>
     </sheetView>
@@ -27794,7 +27794,7 @@
     <col min="8" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>1300</v>
       </c>
@@ -27817,7 +27817,7 @@
         <v>2190</v>
       </c>
     </row>
-    <row r="2" spans="1:7" s="2" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
@@ -27831,7 +27831,7 @@
         <v>1796</v>
       </c>
     </row>
-    <row r="3" spans="1:7" s="2" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>1</v>
       </c>
@@ -27845,7 +27845,7 @@
         <v>1796</v>
       </c>
     </row>
-    <row r="4" spans="1:7" s="2" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>2</v>
       </c>
@@ -27859,7 +27859,7 @@
         <v>1796</v>
       </c>
     </row>
-    <row r="5" spans="1:7" s="2" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>3</v>
       </c>
@@ -27873,7 +27873,7 @@
         <v>1796</v>
       </c>
     </row>
-    <row r="6" spans="1:7" s="2" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>4</v>
       </c>
@@ -27887,7 +27887,7 @@
         <v>1796</v>
       </c>
     </row>
-    <row r="7" spans="1:7" s="2" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>5</v>
       </c>
@@ -27901,7 +27901,7 @@
         <v>1796</v>
       </c>
     </row>
-    <row r="8" spans="1:7" s="2" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>6</v>
       </c>
@@ -27915,7 +27915,7 @@
         <v>1796</v>
       </c>
     </row>
-    <row r="9" spans="1:7" s="2" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>7</v>
       </c>
@@ -27929,7 +27929,7 @@
         <v>1796</v>
       </c>
     </row>
-    <row r="10" spans="1:7" s="2" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>8</v>
       </c>
@@ -27943,7 +27943,7 @@
         <v>1796</v>
       </c>
     </row>
-    <row r="11" spans="1:7" s="2" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>9</v>
       </c>
@@ -27957,7 +27957,7 @@
         <v>1796</v>
       </c>
     </row>
-    <row r="12" spans="1:7" s="2" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>10</v>
       </c>
@@ -27971,7 +27971,7 @@
         <v>1796</v>
       </c>
     </row>
-    <row r="13" spans="1:7" s="2" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>11</v>
       </c>
@@ -27985,7 +27985,7 @@
         <v>1796</v>
       </c>
     </row>
-    <row r="14" spans="1:7" s="2" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>12</v>
       </c>
@@ -27999,7 +27999,7 @@
         <v>1796</v>
       </c>
     </row>
-    <row r="15" spans="1:7" s="2" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>13</v>
       </c>
@@ -28013,7 +28013,7 @@
         <v>1796</v>
       </c>
     </row>
-    <row r="16" spans="1:7" s="2" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
         <v>14</v>
       </c>
@@ -28027,7 +28027,7 @@
         <v>1796</v>
       </c>
     </row>
-    <row r="17" spans="1:7" s="2" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
         <v>15</v>
       </c>
@@ -28041,7 +28041,7 @@
         <v>1796</v>
       </c>
     </row>
-    <row r="18" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
         <v>16</v>
       </c>
@@ -28055,7 +28055,7 @@
         <v>2210</v>
       </c>
     </row>
-    <row r="19" spans="1:7" s="2" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
         <v>17</v>
       </c>
@@ -28069,7 +28069,7 @@
         <v>1796</v>
       </c>
     </row>
-    <row r="20" spans="1:7" s="2" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
         <v>18</v>
       </c>
@@ -28083,7 +28083,7 @@
         <v>1796</v>
       </c>
     </row>
-    <row r="21" spans="1:7" s="2" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
         <v>20</v>
       </c>
@@ -28097,7 +28097,7 @@
         <v>1796</v>
       </c>
     </row>
-    <row r="22" spans="1:7" s="2" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
         <v>21</v>
       </c>
@@ -28111,7 +28111,7 @@
         <v>1796</v>
       </c>
     </row>
-    <row r="23" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
         <v>2072</v>
       </c>
@@ -28128,7 +28128,7 @@
         <v>2210</v>
       </c>
     </row>
-    <row r="24" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
         <v>2073</v>
       </c>
@@ -28145,7 +28145,7 @@
         <v>2210</v>
       </c>
     </row>
-    <row r="25" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
         <v>2074</v>
       </c>
@@ -28162,7 +28162,7 @@
         <v>2210</v>
       </c>
     </row>
-    <row r="26" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
         <v>2075</v>
       </c>
@@ -28179,7 +28179,7 @@
         <v>2210</v>
       </c>
     </row>
-    <row r="27" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
         <v>2076</v>
       </c>
@@ -28196,7 +28196,7 @@
         <v>2210</v>
       </c>
     </row>
-    <row r="28" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
         <v>2077</v>
       </c>
@@ -28213,7 +28213,7 @@
         <v>2210</v>
       </c>
     </row>
-    <row r="29" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
         <v>2078</v>
       </c>
@@ -28230,7 +28230,7 @@
         <v>2210</v>
       </c>
     </row>
-    <row r="30" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
         <v>2079</v>
       </c>
@@ -28247,7 +28247,7 @@
         <v>2210</v>
       </c>
     </row>
-    <row r="31" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
         <v>2080</v>
       </c>
@@ -28264,7 +28264,7 @@
         <v>2210</v>
       </c>
     </row>
-    <row r="32" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
         <v>2081</v>
       </c>
@@ -28281,7 +28281,7 @@
         <v>2210</v>
       </c>
     </row>
-    <row r="33" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33" s="2" t="s">
         <v>2082</v>
       </c>
@@ -28298,7 +28298,7 @@
         <v>2210</v>
       </c>
     </row>
-    <row r="34" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34" s="2" t="s">
         <v>2083</v>
       </c>
@@ -28315,7 +28315,7 @@
         <v>2210</v>
       </c>
     </row>
-    <row r="35" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35" s="2" t="s">
         <v>2084</v>
       </c>
@@ -28332,7 +28332,7 @@
         <v>2210</v>
       </c>
     </row>
-    <row r="36" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36" s="2" t="s">
         <v>2085</v>
       </c>
@@ -28349,7 +28349,7 @@
         <v>2210</v>
       </c>
     </row>
-    <row r="37" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A37" s="2" t="s">
         <v>2086</v>
       </c>
@@ -28366,7 +28366,7 @@
         <v>2210</v>
       </c>
     </row>
-    <row r="38" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A38" s="2" t="s">
         <v>2087</v>
       </c>
@@ -28383,7 +28383,7 @@
         <v>2210</v>
       </c>
     </row>
-    <row r="39" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A39" s="2" t="s">
         <v>2088</v>
       </c>
@@ -28400,7 +28400,7 @@
         <v>2210</v>
       </c>
     </row>
-    <row r="40" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A40" s="2" t="s">
         <v>2089</v>
       </c>
@@ -28417,7 +28417,7 @@
         <v>2210</v>
       </c>
     </row>
-    <row r="41" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A41" s="2" t="s">
         <v>2090</v>
       </c>
@@ -28434,7 +28434,7 @@
         <v>2210</v>
       </c>
     </row>
-    <row r="42" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A42" s="2" t="s">
         <v>2091</v>
       </c>
@@ -28451,7 +28451,7 @@
         <v>2210</v>
       </c>
     </row>
-    <row r="43" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A43" s="2" t="s">
         <v>2092</v>
       </c>
@@ -28468,7 +28468,7 @@
         <v>2210</v>
       </c>
     </row>
-    <row r="44" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A44" s="2" t="s">
         <v>2093</v>
       </c>
@@ -28485,7 +28485,7 @@
         <v>2210</v>
       </c>
     </row>
-    <row r="45" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A45" s="2" t="s">
         <v>2094</v>
       </c>
@@ -28502,7 +28502,7 @@
         <v>2210</v>
       </c>
     </row>
-    <row r="46" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A46" s="2" t="s">
         <v>2095</v>
       </c>
@@ -28519,7 +28519,7 @@
         <v>2210</v>
       </c>
     </row>
-    <row r="47" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A47" s="2" t="s">
         <v>2096</v>
       </c>
@@ -28536,7 +28536,7 @@
         <v>2210</v>
       </c>
     </row>
-    <row r="48" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A48" s="2" t="s">
         <v>2097</v>
       </c>
@@ -28553,7 +28553,7 @@
         <v>2210</v>
       </c>
     </row>
-    <row r="49" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A49" s="2" t="s">
         <v>2098</v>
       </c>
@@ -28570,7 +28570,7 @@
         <v>2210</v>
       </c>
     </row>
-    <row r="50" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A50" s="2" t="s">
         <v>2099</v>
       </c>
@@ -28587,7 +28587,7 @@
         <v>2210</v>
       </c>
     </row>
-    <row r="51" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A51" s="2" t="s">
         <v>2100</v>
       </c>
@@ -28604,7 +28604,7 @@
         <v>2210</v>
       </c>
     </row>
-    <row r="52" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A52" s="2" t="s">
         <v>2101</v>
       </c>
@@ -28621,7 +28621,7 @@
         <v>2210</v>
       </c>
     </row>
-    <row r="53" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A53" s="2" t="s">
         <v>2102</v>
       </c>
@@ -28638,7 +28638,7 @@
         <v>2210</v>
       </c>
     </row>
-    <row r="54" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A54" s="2" t="s">
         <v>2103</v>
       </c>
@@ -28655,7 +28655,7 @@
         <v>2210</v>
       </c>
     </row>
-    <row r="55" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A55" s="2" t="s">
         <v>2104</v>
       </c>
@@ -28672,7 +28672,7 @@
         <v>2210</v>
       </c>
     </row>
-    <row r="56" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A56" s="2" t="s">
         <v>2105</v>
       </c>
@@ -28689,7 +28689,7 @@
         <v>2210</v>
       </c>
     </row>
-    <row r="57" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A57" s="2" t="s">
         <v>2106</v>
       </c>
@@ -28706,7 +28706,7 @@
         <v>2210</v>
       </c>
     </row>
-    <row r="58" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A58" s="2" t="s">
         <v>2107</v>
       </c>
@@ -28723,7 +28723,7 @@
         <v>2210</v>
       </c>
     </row>
-    <row r="59" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A59" s="2" t="s">
         <v>2108</v>
       </c>
@@ -28740,7 +28740,7 @@
         <v>2210</v>
       </c>
     </row>
-    <row r="60" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A60" s="2" t="s">
         <v>2109</v>
       </c>
@@ -28757,7 +28757,7 @@
         <v>2210</v>
       </c>
     </row>
-    <row r="61" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A61" s="2" t="s">
         <v>2110</v>
       </c>
@@ -28774,7 +28774,7 @@
         <v>2210</v>
       </c>
     </row>
-    <row r="62" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A62" s="2" t="s">
         <v>2111</v>
       </c>
@@ -28791,7 +28791,7 @@
         <v>2210</v>
       </c>
     </row>
-    <row r="63" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A63" s="2" t="s">
         <v>2112</v>
       </c>
@@ -28808,7 +28808,7 @@
         <v>2210</v>
       </c>
     </row>
-    <row r="64" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A64" s="2" t="s">
         <v>2113</v>
       </c>
@@ -28825,7 +28825,7 @@
         <v>2210</v>
       </c>
     </row>
-    <row r="65" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A65" s="2" t="s">
         <v>2114</v>
       </c>
@@ -28842,7 +28842,7 @@
         <v>2210</v>
       </c>
     </row>
-    <row r="66" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A66" s="2" t="s">
         <v>2115</v>
       </c>
@@ -28859,7 +28859,7 @@
         <v>2210</v>
       </c>
     </row>
-    <row r="67" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A67" s="2" t="s">
         <v>2116</v>
       </c>
@@ -28876,7 +28876,7 @@
         <v>2210</v>
       </c>
     </row>
-    <row r="68" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A68" s="2" t="s">
         <v>2117</v>
       </c>
@@ -28893,7 +28893,7 @@
         <v>2210</v>
       </c>
     </row>
-    <row r="69" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A69" s="2" t="s">
         <v>2118</v>
       </c>
@@ -28910,7 +28910,7 @@
         <v>2210</v>
       </c>
     </row>
-    <row r="70" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A70" s="2" t="s">
         <v>2119</v>
       </c>
@@ -28927,7 +28927,7 @@
         <v>2210</v>
       </c>
     </row>
-    <row r="71" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A71" s="2" t="s">
         <v>2120</v>
       </c>
@@ -28944,7 +28944,7 @@
         <v>2210</v>
       </c>
     </row>
-    <row r="72" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A72" s="2" t="s">
         <v>2121</v>
       </c>
@@ -28961,7 +28961,7 @@
         <v>2210</v>
       </c>
     </row>
-    <row r="73" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A73" s="2" t="s">
         <v>2122</v>
       </c>
@@ -28978,7 +28978,7 @@
         <v>2210</v>
       </c>
     </row>
-    <row r="74" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A74" s="2" t="s">
         <v>2123</v>
       </c>
@@ -28995,7 +28995,7 @@
         <v>2210</v>
       </c>
     </row>
-    <row r="75" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A75" s="2" t="s">
         <v>2124</v>
       </c>
@@ -29012,7 +29012,7 @@
         <v>2210</v>
       </c>
     </row>
-    <row r="76" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A76" s="2" t="s">
         <v>2125</v>
       </c>
@@ -29029,7 +29029,7 @@
         <v>2210</v>
       </c>
     </row>
-    <row r="77" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A77" s="2" t="s">
         <v>2126</v>
       </c>
@@ -29046,7 +29046,7 @@
         <v>2210</v>
       </c>
     </row>
-    <row r="78" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A78" s="2" t="s">
         <v>2127</v>
       </c>
@@ -29063,7 +29063,7 @@
         <v>2210</v>
       </c>
     </row>
-    <row r="79" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A79" s="2" t="s">
         <v>2128</v>
       </c>
@@ -29080,7 +29080,7 @@
         <v>2210</v>
       </c>
     </row>
-    <row r="80" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A80" s="2" t="s">
         <v>2129</v>
       </c>
@@ -29097,7 +29097,7 @@
         <v>2210</v>
       </c>
     </row>
-    <row r="81" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A81" s="2" t="s">
         <v>2130</v>
       </c>
@@ -29114,7 +29114,7 @@
         <v>2210</v>
       </c>
     </row>
-    <row r="82" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A82" s="2" t="s">
         <v>2131</v>
       </c>
@@ -29131,7 +29131,7 @@
         <v>2210</v>
       </c>
     </row>
-    <row r="83" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A83" s="2" t="s">
         <v>2132</v>
       </c>
@@ -29148,7 +29148,7 @@
         <v>2210</v>
       </c>
     </row>
-    <row r="84" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A84" s="2" t="s">
         <v>2133</v>
       </c>
@@ -29165,7 +29165,7 @@
         <v>2210</v>
       </c>
     </row>
-    <row r="85" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A85" s="2" t="s">
         <v>2134</v>
       </c>
@@ -29182,7 +29182,7 @@
         <v>2210</v>
       </c>
     </row>
-    <row r="86" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A86" s="2" t="s">
         <v>2135</v>
       </c>
@@ -29199,7 +29199,7 @@
         <v>2210</v>
       </c>
     </row>
-    <row r="87" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A87" s="2" t="s">
         <v>2136</v>
       </c>
@@ -29216,7 +29216,7 @@
         <v>2210</v>
       </c>
     </row>
-    <row r="88" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A88" s="2" t="s">
         <v>2137</v>
       </c>
@@ -29233,7 +29233,7 @@
         <v>2210</v>
       </c>
     </row>
-    <row r="89" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A89" s="2" t="s">
         <v>2138</v>
       </c>
@@ -29250,7 +29250,7 @@
         <v>2210</v>
       </c>
     </row>
-    <row r="90" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A90" s="2" t="s">
         <v>2139</v>
       </c>
@@ -29267,7 +29267,7 @@
         <v>2210</v>
       </c>
     </row>
-    <row r="91" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A91" s="2" t="s">
         <v>2140</v>
       </c>
@@ -29284,7 +29284,7 @@
         <v>2210</v>
       </c>
     </row>
-    <row r="92" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A92" s="2" t="s">
         <v>2141</v>
       </c>
@@ -29301,7 +29301,7 @@
         <v>2210</v>
       </c>
     </row>
-    <row r="93" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A93" s="2" t="s">
         <v>2142</v>
       </c>
@@ -29318,7 +29318,7 @@
         <v>2210</v>
       </c>
     </row>
-    <row r="94" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A94" s="2" t="s">
         <v>2143</v>
       </c>
@@ -29335,7 +29335,7 @@
         <v>2210</v>
       </c>
     </row>
-    <row r="95" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A95" s="2" t="s">
         <v>2144</v>
       </c>
@@ -29352,7 +29352,7 @@
         <v>2210</v>
       </c>
     </row>
-    <row r="96" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A96" s="2" t="s">
         <v>2145</v>
       </c>
@@ -29369,7 +29369,7 @@
         <v>2210</v>
       </c>
     </row>
-    <row r="97" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A97" s="2" t="s">
         <v>2146</v>
       </c>
@@ -29386,7 +29386,7 @@
         <v>2210</v>
       </c>
     </row>
-    <row r="98" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A98" s="2" t="s">
         <v>2147</v>
       </c>
@@ -29403,7 +29403,7 @@
         <v>2210</v>
       </c>
     </row>
-    <row r="99" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A99" s="2" t="s">
         <v>2148</v>
       </c>
@@ -29420,7 +29420,7 @@
         <v>2210</v>
       </c>
     </row>
-    <row r="100" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A100" s="2" t="s">
         <v>2149</v>
       </c>
@@ -29437,7 +29437,7 @@
         <v>2210</v>
       </c>
     </row>
-    <row r="101" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A101" s="2" t="s">
         <v>2150</v>
       </c>
@@ -29454,7 +29454,7 @@
         <v>2210</v>
       </c>
     </row>
-    <row r="102" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A102" s="2" t="s">
         <v>2151</v>
       </c>
@@ -29471,7 +29471,7 @@
         <v>2210</v>
       </c>
     </row>
-    <row r="103" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A103" s="2" t="s">
         <v>2152</v>
       </c>
@@ -29488,7 +29488,7 @@
         <v>2210</v>
       </c>
     </row>
-    <row r="104" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A104" s="2" t="s">
         <v>2153</v>
       </c>
@@ -29505,7 +29505,7 @@
         <v>2210</v>
       </c>
     </row>
-    <row r="105" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A105" s="2" t="s">
         <v>2154</v>
       </c>
@@ -29522,7 +29522,7 @@
         <v>2210</v>
       </c>
     </row>
-    <row r="106" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A106" s="2" t="s">
         <v>2155</v>
       </c>
@@ -29539,7 +29539,7 @@
         <v>2210</v>
       </c>
     </row>
-    <row r="107" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A107" s="2" t="s">
         <v>2156</v>
       </c>
@@ -29556,7 +29556,7 @@
         <v>2210</v>
       </c>
     </row>
-    <row r="108" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A108" s="2" t="s">
         <v>2157</v>
       </c>
@@ -29573,7 +29573,7 @@
         <v>2210</v>
       </c>
     </row>
-    <row r="109" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A109" s="2" t="s">
         <v>2158</v>
       </c>
@@ -29590,7 +29590,7 @@
         <v>2210</v>
       </c>
     </row>
-    <row r="110" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A110" s="2" t="s">
         <v>2159</v>
       </c>
@@ -29607,7 +29607,7 @@
         <v>2210</v>
       </c>
     </row>
-    <row r="111" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A111" s="2" t="s">
         <v>2160</v>
       </c>
@@ -29624,7 +29624,7 @@
         <v>2210</v>
       </c>
     </row>
-    <row r="112" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A112" s="2" t="s">
         <v>2161</v>
       </c>
@@ -29641,7 +29641,7 @@
         <v>2210</v>
       </c>
     </row>
-    <row r="113" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A113" s="2" t="s">
         <v>2162</v>
       </c>
@@ -29655,7 +29655,7 @@
         <v>2210</v>
       </c>
     </row>
-    <row r="114" spans="1:7" s="2" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A114" s="2" t="s">
         <v>2163</v>
       </c>
@@ -29669,7 +29669,7 @@
         <v>1796</v>
       </c>
     </row>
-    <row r="115" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A115" s="2" t="s">
         <v>2164</v>
       </c>

</xml_diff>

<commit_message>
Add TIMSS 2019 G8 PVs
</commit_message>
<xml_diff>
--- a/2_TIMSS_2019_G4_clean/Instructions.xlsx
+++ b/2_TIMSS_2019_G4_clean/Instructions.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\TIMSS_2019\2_TIMSS_2019_G4_clean\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9866A97C-1D25-42C9-87FB-BD87012FCBD1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB5F65AD-19EF-41EB-9BE1-59B5C0D978D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-23148" yWindow="4284" windowWidth="23256" windowHeight="12576" tabRatio="730" activeTab="2" xr2:uid="{6A18A5C5-ACE7-445C-877F-08C8BDB6A624}"/>
+    <workbookView xWindow="-23148" yWindow="4284" windowWidth="23256" windowHeight="12576" tabRatio="730" activeTab="5" xr2:uid="{6A18A5C5-ACE7-445C-877F-08C8BDB6A624}"/>
   </bookViews>
   <sheets>
     <sheet name="1_G4_PV" sheetId="14" r:id="rId1"/>
@@ -46,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8690" uniqueCount="3661">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8691" uniqueCount="3666">
   <si>
     <t>IDCNTRY</t>
   </si>
@@ -11029,6 +11029,21 @@
   </si>
   <si>
     <t>(1=5) (2=4) (3=3) (4=2) (5=1) (6=0)</t>
+  </si>
+  <si>
+    <t>SCLComSE</t>
+  </si>
+  <si>
+    <t>IDXComSE</t>
+  </si>
+  <si>
+    <t>MSCHdMate</t>
+  </si>
+  <si>
+    <t>MSCHdSubj</t>
+  </si>
+  <si>
+    <t>SPSS file: SCIWGT</t>
   </si>
 </sst>
 </file>
@@ -11052,7 +11067,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -11062,6 +11077,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="1"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -11078,7 +11099,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -11091,6 +11112,15 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -20226,9 +20256,9 @@
   </sheetPr>
   <dimension ref="A1:G145"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A129" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D135" sqref="D135"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -21561,7 +21591,7 @@
       <c r="B58" s="2" t="s">
         <v>1732</v>
       </c>
-      <c r="C58" s="2" t="s">
+      <c r="C58" s="6" t="s">
         <v>1734</v>
       </c>
       <c r="D58" s="2" t="s">
@@ -21584,8 +21614,8 @@
       <c r="B59" s="2" t="s">
         <v>1732</v>
       </c>
-      <c r="C59" s="2" t="s">
-        <v>1735</v>
+      <c r="C59" s="5" t="s">
+        <v>3663</v>
       </c>
       <c r="D59" s="2" t="s">
         <v>1036</v>
@@ -21607,7 +21637,7 @@
       <c r="B60" s="2" t="s">
         <v>1732</v>
       </c>
-      <c r="C60" s="2" t="s">
+      <c r="C60" s="6" t="s">
         <v>1739</v>
       </c>
       <c r="D60" s="2" t="s">
@@ -21630,7 +21660,7 @@
       <c r="B61" s="2" t="s">
         <v>1732</v>
       </c>
-      <c r="C61" s="2" t="s">
+      <c r="C61" s="6" t="s">
         <v>1737</v>
       </c>
       <c r="D61" s="2" t="s">
@@ -21653,7 +21683,7 @@
       <c r="B62" s="2" t="s">
         <v>1732</v>
       </c>
-      <c r="C62" s="2" t="s">
+      <c r="C62" s="6" t="s">
         <v>1741</v>
       </c>
       <c r="D62" s="2" t="s">
@@ -21676,7 +21706,7 @@
       <c r="B63" s="2" t="s">
         <v>1732</v>
       </c>
-      <c r="C63" s="2" t="s">
+      <c r="C63" s="6" t="s">
         <v>1738</v>
       </c>
       <c r="D63" s="2" t="s">
@@ -21699,7 +21729,7 @@
       <c r="B64" s="2" t="s">
         <v>1732</v>
       </c>
-      <c r="C64" s="2" t="s">
+      <c r="C64" s="6" t="s">
         <v>1736</v>
       </c>
       <c r="D64" s="2" t="s">
@@ -21722,8 +21752,8 @@
       <c r="B65" s="2" t="s">
         <v>1732</v>
       </c>
-      <c r="C65" s="2" t="s">
-        <v>1735</v>
+      <c r="C65" s="5" t="s">
+        <v>3664</v>
       </c>
       <c r="D65" s="2" t="s">
         <v>1042</v>
@@ -21745,7 +21775,7 @@
       <c r="B66" s="2" t="s">
         <v>1732</v>
       </c>
-      <c r="C66" s="2" t="s">
+      <c r="C66" s="6" t="s">
         <v>1740</v>
       </c>
       <c r="D66" s="2" t="s">
@@ -22791,7 +22821,7 @@
       <c r="B112" s="2" t="s">
         <v>1667</v>
       </c>
-      <c r="C112" s="2" t="s">
+      <c r="C112" s="5" t="s">
         <v>1666</v>
       </c>
       <c r="D112" s="2" t="s">
@@ -23174,238 +23204,238 @@
         <v>2209</v>
       </c>
     </row>
-    <row r="133" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A133" s="2" t="s">
+    <row r="133" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A133" s="6" t="s">
         <v>457</v>
       </c>
-      <c r="B133" s="2" t="s">
+      <c r="B133" s="6" t="s">
         <v>2039</v>
       </c>
-      <c r="C133" s="2" t="s">
+      <c r="C133" s="6" t="s">
         <v>1809</v>
       </c>
-      <c r="D133" s="2" t="s">
+      <c r="D133" s="6" t="s">
         <v>1110</v>
       </c>
-      <c r="F133" s="3">
+      <c r="F133" s="7">
         <v>999999</v>
       </c>
-      <c r="G133" s="2" t="s">
+      <c r="G133" s="6" t="s">
         <v>2210</v>
       </c>
     </row>
-    <row r="134" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A134" s="2" t="s">
+    <row r="134" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A134" s="6" t="s">
         <v>458</v>
       </c>
-      <c r="B134" s="2" t="s">
+      <c r="B134" s="6" t="s">
         <v>2039</v>
       </c>
-      <c r="C134" s="2" t="s">
+      <c r="C134" s="6" t="s">
         <v>1810</v>
       </c>
-      <c r="D134" s="2" t="s">
+      <c r="D134" s="6" t="s">
         <v>1111</v>
       </c>
-      <c r="E134" s="2" t="s">
+      <c r="E134" s="6" t="s">
         <v>1472</v>
       </c>
-      <c r="F134" s="3">
-        <v>9</v>
-      </c>
-      <c r="G134" s="2" t="s">
-        <v>2209</v>
-      </c>
-    </row>
-    <row r="135" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A135" s="2" t="s">
+      <c r="F134" s="7">
+        <v>9</v>
+      </c>
+      <c r="G134" s="6" t="s">
+        <v>2209</v>
+      </c>
+    </row>
+    <row r="135" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A135" s="6" t="s">
         <v>459</v>
       </c>
-      <c r="B135" s="2" t="s">
+      <c r="B135" s="6" t="s">
         <v>2040</v>
       </c>
-      <c r="C135" s="2" t="s">
+      <c r="C135" s="6" t="s">
         <v>1811</v>
       </c>
-      <c r="D135" s="2" t="s">
+      <c r="D135" s="6" t="s">
         <v>1112</v>
       </c>
-      <c r="F135" s="3">
+      <c r="F135" s="7">
         <v>999999</v>
       </c>
-      <c r="G135" s="2" t="s">
+      <c r="G135" s="6" t="s">
         <v>2210</v>
       </c>
     </row>
-    <row r="136" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A136" s="2" t="s">
+    <row r="136" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A136" s="6" t="s">
         <v>460</v>
       </c>
-      <c r="B136" s="2" t="s">
+      <c r="B136" s="6" t="s">
         <v>2040</v>
       </c>
-      <c r="C136" s="2" t="s">
+      <c r="C136" s="6" t="s">
         <v>1812</v>
       </c>
-      <c r="D136" s="2" t="s">
+      <c r="D136" s="6" t="s">
         <v>1113</v>
       </c>
-      <c r="E136" s="2" t="s">
+      <c r="E136" s="6" t="s">
         <v>1472</v>
       </c>
-      <c r="F136" s="3">
-        <v>9</v>
-      </c>
-      <c r="G136" s="2" t="s">
-        <v>2209</v>
-      </c>
-    </row>
-    <row r="137" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A137" s="2" t="s">
+      <c r="F136" s="7">
+        <v>9</v>
+      </c>
+      <c r="G136" s="6" t="s">
+        <v>2209</v>
+      </c>
+    </row>
+    <row r="137" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A137" s="6" t="s">
         <v>461</v>
       </c>
-      <c r="B137" s="2" t="s">
+      <c r="B137" s="6" t="s">
         <v>2041</v>
       </c>
-      <c r="C137" s="2" t="s">
+      <c r="C137" s="6" t="s">
         <v>1813</v>
       </c>
-      <c r="D137" s="2" t="s">
+      <c r="D137" s="6" t="s">
         <v>1114</v>
       </c>
-      <c r="F137" s="3">
+      <c r="F137" s="7">
         <v>999999</v>
       </c>
-      <c r="G137" s="2" t="s">
+      <c r="G137" s="6" t="s">
         <v>2210</v>
       </c>
     </row>
-    <row r="138" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A138" s="2" t="s">
+    <row r="138" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A138" s="6" t="s">
         <v>462</v>
       </c>
-      <c r="B138" s="2" t="s">
+      <c r="B138" s="6" t="s">
         <v>2041</v>
       </c>
-      <c r="C138" s="2" t="s">
+      <c r="C138" s="6" t="s">
         <v>1814</v>
       </c>
-      <c r="D138" s="2" t="s">
+      <c r="D138" s="6" t="s">
         <v>1115</v>
       </c>
-      <c r="E138" s="2" t="s">
+      <c r="E138" s="6" t="s">
         <v>1472</v>
       </c>
-      <c r="F138" s="3">
-        <v>9</v>
-      </c>
-      <c r="G138" s="2" t="s">
-        <v>2209</v>
-      </c>
-    </row>
-    <row r="139" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A139" s="2" t="s">
+      <c r="F138" s="7">
+        <v>9</v>
+      </c>
+      <c r="G138" s="6" t="s">
+        <v>2209</v>
+      </c>
+    </row>
+    <row r="139" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A139" s="6" t="s">
         <v>463</v>
       </c>
-      <c r="B139" s="2" t="s">
+      <c r="B139" s="6" t="s">
         <v>3412</v>
       </c>
-      <c r="C139" s="2" t="s">
+      <c r="C139" s="6" t="s">
         <v>1815</v>
       </c>
-      <c r="D139" s="2" t="s">
+      <c r="D139" s="6" t="s">
         <v>1116</v>
       </c>
-      <c r="F139" s="3">
+      <c r="F139" s="7">
         <v>999999</v>
       </c>
-      <c r="G139" s="2" t="s">
+      <c r="G139" s="6" t="s">
         <v>2210</v>
       </c>
     </row>
-    <row r="140" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A140" s="2" t="s">
+    <row r="140" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A140" s="6" t="s">
         <v>464</v>
       </c>
-      <c r="B140" s="2" t="s">
+      <c r="B140" s="6" t="s">
         <v>3412</v>
       </c>
-      <c r="C140" s="2" t="s">
+      <c r="C140" s="6" t="s">
         <v>1816</v>
       </c>
-      <c r="D140" s="2" t="s">
+      <c r="D140" s="6" t="s">
         <v>1117</v>
       </c>
-      <c r="E140" s="2" t="s">
+      <c r="E140" s="6" t="s">
         <v>1472</v>
       </c>
-      <c r="F140" s="3">
-        <v>9</v>
-      </c>
-      <c r="G140" s="2" t="s">
-        <v>2209</v>
-      </c>
-    </row>
-    <row r="141" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A141" s="2" t="s">
+      <c r="F140" s="7">
+        <v>9</v>
+      </c>
+      <c r="G140" s="6" t="s">
+        <v>2209</v>
+      </c>
+    </row>
+    <row r="141" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A141" s="6" t="s">
         <v>465</v>
       </c>
-      <c r="B141" s="2" t="s">
+      <c r="B141" s="6" t="s">
         <v>2043</v>
       </c>
-      <c r="C141" s="2" t="s">
-        <v>1818</v>
-      </c>
-      <c r="D141" s="2" t="s">
+      <c r="C141" s="5" t="s">
+        <v>3661</v>
+      </c>
+      <c r="D141" s="6" t="s">
         <v>1118</v>
       </c>
-      <c r="F141" s="3">
+      <c r="F141" s="7">
         <v>999999</v>
       </c>
-      <c r="G141" s="2" t="s">
+      <c r="G141" s="6" t="s">
         <v>2210</v>
       </c>
     </row>
-    <row r="142" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A142" s="2" t="s">
+    <row r="142" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A142" s="6" t="s">
         <v>466</v>
       </c>
-      <c r="B142" s="2" t="s">
+      <c r="B142" s="6" t="s">
         <v>2043</v>
       </c>
-      <c r="C142" s="2" t="s">
-        <v>1817</v>
-      </c>
-      <c r="D142" s="2" t="s">
+      <c r="C142" s="5" t="s">
+        <v>3662</v>
+      </c>
+      <c r="D142" s="6" t="s">
         <v>1119</v>
       </c>
-      <c r="E142" s="2" t="s">
+      <c r="E142" s="6" t="s">
         <v>1472</v>
       </c>
-      <c r="F142" s="3">
-        <v>9</v>
-      </c>
-      <c r="G142" s="2" t="s">
-        <v>2209</v>
-      </c>
-    </row>
-    <row r="143" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A143" s="2" t="s">
+      <c r="F142" s="7">
+        <v>9</v>
+      </c>
+      <c r="G142" s="6" t="s">
+        <v>2209</v>
+      </c>
+    </row>
+    <row r="143" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A143" s="6" t="s">
         <v>467</v>
       </c>
-      <c r="B143" s="2" t="s">
+      <c r="B143" s="6" t="s">
         <v>1120</v>
       </c>
-      <c r="C143" s="2" t="s">
+      <c r="C143" s="6" t="s">
         <v>1819</v>
       </c>
-      <c r="D143" s="2" t="s">
+      <c r="D143" s="6" t="s">
         <v>1120</v>
       </c>
-      <c r="F143" s="3">
-        <v>9</v>
-      </c>
-      <c r="G143" s="2" t="s">
+      <c r="F143" s="7">
+        <v>9</v>
+      </c>
+      <c r="G143" s="6" t="s">
         <v>2210</v>
       </c>
     </row>
@@ -27777,9 +27807,9 @@
   </sheetPr>
   <dimension ref="A1:G115"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A102" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B114" sqref="B114"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -28070,10 +28100,13 @@
       </c>
     </row>
     <row r="20" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A20" s="2" t="s">
+      <c r="A20" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="D20" s="2" t="s">
+      <c r="B20" s="5" t="s">
+        <v>3665</v>
+      </c>
+      <c r="D20" s="5" t="s">
         <v>674</v>
       </c>
       <c r="F20" s="3">

</xml_diff>

<commit_message>
Complete TIMSS 2019 data cleaning DRAFT
</commit_message>
<xml_diff>
--- a/2_TIMSS_2019_G4_clean/Instructions.xlsx
+++ b/2_TIMSS_2019_G4_clean/Instructions.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\TIMSS_2019\2_TIMSS_2019_G4_clean\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB5F65AD-19EF-41EB-9BE1-59B5C0D978D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7DC5E06E-99EE-49F9-B6C0-F4D2E27266DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-23148" yWindow="4284" windowWidth="23256" windowHeight="12576" tabRatio="730" activeTab="5" xr2:uid="{6A18A5C5-ACE7-445C-877F-08C8BDB6A624}"/>
+    <workbookView xWindow="-23148" yWindow="4284" windowWidth="23256" windowHeight="12576" tabRatio="730" activeTab="2" xr2:uid="{6A18A5C5-ACE7-445C-877F-08C8BDB6A624}"/>
   </bookViews>
   <sheets>
     <sheet name="1_G4_PV" sheetId="14" r:id="rId1"/>
@@ -46,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8691" uniqueCount="3666">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8691" uniqueCount="3667">
   <si>
     <t>IDCNTRY</t>
   </si>
@@ -11044,6 +11044,9 @@
   </si>
   <si>
     <t>SPSS file: SCIWGT</t>
+  </si>
+  <si>
+    <t>SCLBully</t>
   </si>
 </sst>
 </file>
@@ -11067,7 +11070,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -11086,6 +11089,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -11099,7 +11108,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -11121,6 +11130,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -13134,8 +13146,8 @@
   <dimension ref="A1:G86"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E33" sqref="E33"/>
+      <pane ySplit="1" topLeftCell="A59" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C78" sqref="C78"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -15114,8 +15126,8 @@
   <dimension ref="A1:G225"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft"/>
+      <pane ySplit="1" topLeftCell="A201" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C208" sqref="C208"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -20256,9 +20268,9 @@
   </sheetPr>
   <dimension ref="A1:G145"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A129" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D135" sqref="D135"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A104" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E109" sqref="E109"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -22821,7 +22833,7 @@
       <c r="B112" s="2" t="s">
         <v>1667</v>
       </c>
-      <c r="C112" s="5" t="s">
+      <c r="C112" s="8" t="s">
         <v>1666</v>
       </c>
       <c r="D112" s="2" t="s">
@@ -23082,8 +23094,8 @@
       <c r="B127" s="2" t="s">
         <v>2036</v>
       </c>
-      <c r="C127" s="2" t="s">
-        <v>1801</v>
+      <c r="C127" s="5" t="s">
+        <v>3666</v>
       </c>
       <c r="D127" s="2" t="s">
         <v>1104</v>
@@ -25752,8 +25764,8 @@
   <dimension ref="A1:G90"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft"/>
+      <pane ySplit="1" topLeftCell="A75" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C83" sqref="C83"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -27807,8 +27819,8 @@
   </sheetPr>
   <dimension ref="A1:G115"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A102" activePane="bottomLeft" state="frozen"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A108" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="B114" sqref="B114"/>
     </sheetView>
   </sheetViews>
@@ -29731,8 +29743,8 @@
   <dimension ref="A1:G147"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft"/>
+      <pane ySplit="1" topLeftCell="A128" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C135" sqref="C135"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -33095,8 +33107,8 @@
   <dimension ref="A1:G158"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft"/>
+      <pane ySplit="1" topLeftCell="A137" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C144" sqref="C144"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Amend TIMSS 2019 data cleaning files
</commit_message>
<xml_diff>
--- a/2_TIMSS_2019_G4_clean/Instructions.xlsx
+++ b/2_TIMSS_2019_G4_clean/Instructions.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\TIMSS_2019\2_TIMSS_2019_G4_clean\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7DC5E06E-99EE-49F9-B6C0-F4D2E27266DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1CCD625-5FEF-47A2-885D-9D0C98A8E419}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-23148" yWindow="4284" windowWidth="23256" windowHeight="12576" tabRatio="730" activeTab="2" xr2:uid="{6A18A5C5-ACE7-445C-877F-08C8BDB6A624}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="730" activeTab="8" xr2:uid="{6A18A5C5-ACE7-445C-877F-08C8BDB6A624}"/>
   </bookViews>
   <sheets>
     <sheet name="1_G4_PV" sheetId="14" r:id="rId1"/>
@@ -11053,7 +11053,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -11068,6 +11068,19 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Fira Code"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Fira Code"/>
+      <family val="3"/>
     </font>
   </fonts>
   <fills count="5">
@@ -11108,7 +11121,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -11134,6 +11147,13 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -15126,8 +15146,8 @@
   <dimension ref="A1:G225"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A201" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C208" sqref="C208"/>
+      <pane ySplit="1" topLeftCell="A101" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A104" sqref="A104"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -20268,7 +20288,7 @@
   </sheetPr>
   <dimension ref="A1:G145"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A104" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="E109" sqref="E109"/>
     </sheetView>
@@ -23513,7 +23533,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft"/>
+      <selection pane="bottomLeft" activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -36736,30 +36756,30 @@
   </sheetPr>
   <dimension ref="A1:G351"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft"/>
+      <selection pane="bottomLeft" activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="11.5703125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="49" customWidth="1"/>
-    <col min="3" max="3" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.42578125" style="11" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="58.7109375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="26.7109375" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="12.85546875" style="1" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="32.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>1300</v>
       </c>
       <c r="B1" s="4" t="s">
         <v>1318</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="C1" s="9" t="s">
         <v>1302</v>
       </c>
       <c r="D1" s="4" t="s">
@@ -36782,7 +36802,7 @@
       <c r="B2" s="2" t="s">
         <v>1667</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C2" s="10" t="s">
         <v>1666</v>
       </c>
       <c r="D2" s="2" t="s">
@@ -36805,7 +36825,7 @@
       <c r="B3" s="2" t="s">
         <v>1669</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="C3" s="10" t="s">
         <v>1668</v>
       </c>
       <c r="D3" s="2" t="s">
@@ -36828,7 +36848,7 @@
       <c r="B4" s="2" t="s">
         <v>1680</v>
       </c>
-      <c r="C4" s="2" t="s">
+      <c r="C4" s="10" t="s">
         <v>1670</v>
       </c>
       <c r="D4" s="2" t="s">
@@ -36851,7 +36871,7 @@
       <c r="B5" s="2" t="s">
         <v>1681</v>
       </c>
-      <c r="C5" s="2" t="s">
+      <c r="C5" s="10" t="s">
         <v>1671</v>
       </c>
       <c r="D5" s="2" t="s">
@@ -36874,7 +36894,7 @@
       <c r="B6" s="2" t="s">
         <v>1681</v>
       </c>
-      <c r="C6" s="2" t="s">
+      <c r="C6" s="10" t="s">
         <v>1672</v>
       </c>
       <c r="D6" s="2" t="s">
@@ -36897,7 +36917,7 @@
       <c r="B7" s="2" t="s">
         <v>1681</v>
       </c>
-      <c r="C7" s="2" t="s">
+      <c r="C7" s="10" t="s">
         <v>1673</v>
       </c>
       <c r="D7" s="2" t="s">
@@ -36920,7 +36940,7 @@
       <c r="B8" s="2" t="s">
         <v>1681</v>
       </c>
-      <c r="C8" s="2" t="s">
+      <c r="C8" s="10" t="s">
         <v>1674</v>
       </c>
       <c r="D8" s="2" t="s">
@@ -36943,7 +36963,7 @@
       <c r="B9" s="2" t="s">
         <v>1681</v>
       </c>
-      <c r="C9" s="2" t="s">
+      <c r="C9" s="10" t="s">
         <v>1675</v>
       </c>
       <c r="D9" s="2" t="s">
@@ -36966,7 +36986,7 @@
       <c r="B10" s="2" t="s">
         <v>1681</v>
       </c>
-      <c r="C10" s="2" t="s">
+      <c r="C10" s="10" t="s">
         <v>1676</v>
       </c>
       <c r="D10" s="2" t="s">
@@ -36989,7 +37009,7 @@
       <c r="B11" s="2" t="s">
         <v>1681</v>
       </c>
-      <c r="C11" s="2" t="s">
+      <c r="C11" s="10" t="s">
         <v>1677</v>
       </c>
       <c r="D11" s="2" t="s">
@@ -37012,7 +37032,7 @@
       <c r="B12" s="2" t="s">
         <v>1681</v>
       </c>
-      <c r="C12" s="2" t="s">
+      <c r="C12" s="10" t="s">
         <v>1678</v>
       </c>
       <c r="D12" s="2" t="s">
@@ -37035,7 +37055,7 @@
       <c r="B13" s="2" t="s">
         <v>1681</v>
       </c>
-      <c r="C13" s="2" t="s">
+      <c r="C13" s="10" t="s">
         <v>1679</v>
       </c>
       <c r="D13" s="2" t="s">
@@ -37058,7 +37078,7 @@
       <c r="B14" s="2" t="s">
         <v>1915</v>
       </c>
-      <c r="C14" s="2" t="s">
+      <c r="C14" s="10" t="s">
         <v>1913</v>
       </c>
       <c r="D14" s="2" t="s">
@@ -37081,7 +37101,7 @@
       <c r="B15" s="2" t="s">
         <v>1915</v>
       </c>
-      <c r="C15" s="2" t="s">
+      <c r="C15" s="10" t="s">
         <v>1914</v>
       </c>
       <c r="D15" s="2" t="s">
@@ -37104,7 +37124,7 @@
       <c r="B16" s="2" t="s">
         <v>3201</v>
       </c>
-      <c r="C16" s="2" t="s">
+      <c r="C16" s="10" t="s">
         <v>3202</v>
       </c>
       <c r="D16" s="2" t="s">
@@ -37127,7 +37147,7 @@
       <c r="B17" s="2" t="s">
         <v>1684</v>
       </c>
-      <c r="C17" s="2" t="s">
+      <c r="C17" s="10" t="s">
         <v>1682</v>
       </c>
       <c r="D17" s="2" t="s">
@@ -37150,7 +37170,7 @@
       <c r="B18" s="2" t="s">
         <v>1684</v>
       </c>
-      <c r="C18" s="2" t="s">
+      <c r="C18" s="10" t="s">
         <v>1683</v>
       </c>
       <c r="D18" s="2" t="s">
@@ -37173,7 +37193,7 @@
       <c r="B19" s="2" t="s">
         <v>1685</v>
       </c>
-      <c r="C19" s="2" t="s">
+      <c r="C19" s="10" t="s">
         <v>1686</v>
       </c>
       <c r="D19" s="2" t="s">
@@ -37196,7 +37216,7 @@
       <c r="B20" s="2" t="s">
         <v>3203</v>
       </c>
-      <c r="C20" s="2" t="s">
+      <c r="C20" s="10" t="s">
         <v>3204</v>
       </c>
       <c r="D20" s="2" t="s">
@@ -37219,7 +37239,7 @@
       <c r="B21" s="2" t="s">
         <v>1688</v>
       </c>
-      <c r="C21" s="2" t="s">
+      <c r="C21" s="10" t="s">
         <v>1687</v>
       </c>
       <c r="D21" s="2" t="s">
@@ -37242,7 +37262,7 @@
       <c r="B22" s="2" t="s">
         <v>1689</v>
       </c>
-      <c r="C22" s="2" t="s">
+      <c r="C22" s="10" t="s">
         <v>1690</v>
       </c>
       <c r="D22" s="2" t="s">
@@ -37265,7 +37285,7 @@
       <c r="B23" s="2" t="s">
         <v>1689</v>
       </c>
-      <c r="C23" s="2" t="s">
+      <c r="C23" s="10" t="s">
         <v>1691</v>
       </c>
       <c r="D23" s="2" t="s">
@@ -37288,7 +37308,7 @@
       <c r="B24" s="2" t="s">
         <v>3205</v>
       </c>
-      <c r="C24" s="2" t="s">
+      <c r="C24" s="10" t="s">
         <v>3206</v>
       </c>
       <c r="D24" s="2" t="s">
@@ -37311,7 +37331,7 @@
       <c r="B25" s="2" t="s">
         <v>3205</v>
       </c>
-      <c r="C25" s="2" t="s">
+      <c r="C25" s="10" t="s">
         <v>3207</v>
       </c>
       <c r="D25" s="2" t="s">
@@ -37334,7 +37354,7 @@
       <c r="B26" s="2" t="s">
         <v>3205</v>
       </c>
-      <c r="C26" s="2" t="s">
+      <c r="C26" s="10" t="s">
         <v>3208</v>
       </c>
       <c r="D26" s="2" t="s">
@@ -37357,7 +37377,7 @@
       <c r="B27" s="2" t="s">
         <v>3205</v>
       </c>
-      <c r="C27" s="2" t="s">
+      <c r="C27" s="10" t="s">
         <v>3209</v>
       </c>
       <c r="D27" s="2" t="s">
@@ -37380,7 +37400,7 @@
       <c r="B28" s="2" t="s">
         <v>3205</v>
       </c>
-      <c r="C28" s="2" t="s">
+      <c r="C28" s="10" t="s">
         <v>3210</v>
       </c>
       <c r="D28" s="2" t="s">
@@ -37403,7 +37423,7 @@
       <c r="B29" s="2" t="s">
         <v>3205</v>
       </c>
-      <c r="C29" s="2" t="s">
+      <c r="C29" s="10" t="s">
         <v>3211</v>
       </c>
       <c r="D29" s="2" t="s">
@@ -37426,7 +37446,7 @@
       <c r="B30" s="2" t="s">
         <v>1692</v>
       </c>
-      <c r="C30" s="2" t="s">
+      <c r="C30" s="10" t="s">
         <v>1694</v>
       </c>
       <c r="D30" s="2" t="s">
@@ -37449,7 +37469,7 @@
       <c r="B31" s="2" t="s">
         <v>1692</v>
       </c>
-      <c r="C31" s="2" t="s">
+      <c r="C31" s="10" t="s">
         <v>1693</v>
       </c>
       <c r="D31" s="2" t="s">
@@ -37472,7 +37492,7 @@
       <c r="B32" s="2" t="s">
         <v>1692</v>
       </c>
-      <c r="C32" s="2" t="s">
+      <c r="C32" s="10" t="s">
         <v>1695</v>
       </c>
       <c r="D32" s="2" t="s">
@@ -37495,7 +37515,7 @@
       <c r="B33" s="2" t="s">
         <v>1692</v>
       </c>
-      <c r="C33" s="2" t="s">
+      <c r="C33" s="10" t="s">
         <v>1696</v>
       </c>
       <c r="D33" s="2" t="s">
@@ -37518,7 +37538,7 @@
       <c r="B34" s="2" t="s">
         <v>1692</v>
       </c>
-      <c r="C34" s="2" t="s">
+      <c r="C34" s="10" t="s">
         <v>1697</v>
       </c>
       <c r="D34" s="2" t="s">
@@ -37541,7 +37561,7 @@
       <c r="B35" s="2" t="s">
         <v>1698</v>
       </c>
-      <c r="C35" s="2" t="s">
+      <c r="C35" s="10" t="s">
         <v>3212</v>
       </c>
       <c r="D35" s="2" t="s">
@@ -37564,7 +37584,7 @@
       <c r="B36" s="2" t="s">
         <v>1698</v>
       </c>
-      <c r="C36" s="2" t="s">
+      <c r="C36" s="10" t="s">
         <v>1701</v>
       </c>
       <c r="D36" s="2" t="s">
@@ -37587,7 +37607,7 @@
       <c r="B37" s="2" t="s">
         <v>1698</v>
       </c>
-      <c r="C37" s="2" t="s">
+      <c r="C37" s="10" t="s">
         <v>3213</v>
       </c>
       <c r="D37" s="2" t="s">
@@ -37610,7 +37630,7 @@
       <c r="B38" s="2" t="s">
         <v>1698</v>
       </c>
-      <c r="C38" s="2" t="s">
+      <c r="C38" s="10" t="s">
         <v>3214</v>
       </c>
       <c r="D38" s="2" t="s">
@@ -37633,7 +37653,7 @@
       <c r="B39" s="2" t="s">
         <v>1698</v>
       </c>
-      <c r="C39" s="2" t="s">
+      <c r="C39" s="10" t="s">
         <v>3215</v>
       </c>
       <c r="D39" s="2" t="s">
@@ -37656,7 +37676,7 @@
       <c r="B40" s="2" t="s">
         <v>1698</v>
       </c>
-      <c r="C40" s="2" t="s">
+      <c r="C40" s="10" t="s">
         <v>1702</v>
       </c>
       <c r="D40" s="2" t="s">
@@ -37679,7 +37699,7 @@
       <c r="B41" s="2" t="s">
         <v>1698</v>
       </c>
-      <c r="C41" s="2" t="s">
+      <c r="C41" s="10" t="s">
         <v>1705</v>
       </c>
       <c r="D41" s="2" t="s">
@@ -37702,7 +37722,7 @@
       <c r="B42" s="2" t="s">
         <v>1698</v>
       </c>
-      <c r="C42" s="2" t="s">
+      <c r="C42" s="10" t="s">
         <v>1704</v>
       </c>
       <c r="D42" s="2" t="s">
@@ -37725,7 +37745,7 @@
       <c r="B43" s="2" t="s">
         <v>1698</v>
       </c>
-      <c r="C43" s="2" t="s">
+      <c r="C43" s="10" t="s">
         <v>1706</v>
       </c>
       <c r="D43" s="2" t="s">
@@ -37748,7 +37768,7 @@
       <c r="B44" s="2" t="s">
         <v>1698</v>
       </c>
-      <c r="C44" s="2" t="s">
+      <c r="C44" s="10" t="s">
         <v>1707</v>
       </c>
       <c r="D44" s="2" t="s">
@@ -37771,7 +37791,7 @@
       <c r="B45" s="2" t="s">
         <v>1698</v>
       </c>
-      <c r="C45" s="2" t="s">
+      <c r="C45" s="10" t="s">
         <v>1708</v>
       </c>
       <c r="D45" s="2" t="s">
@@ -37794,7 +37814,7 @@
       <c r="B46" s="2" t="s">
         <v>1698</v>
       </c>
-      <c r="C46" s="2" t="s">
+      <c r="C46" s="10" t="s">
         <v>3217</v>
       </c>
       <c r="D46" s="2" t="s">
@@ -37817,7 +37837,7 @@
       <c r="B47" s="2" t="s">
         <v>1698</v>
       </c>
-      <c r="C47" s="2" t="s">
+      <c r="C47" s="10" t="s">
         <v>3219</v>
       </c>
       <c r="D47" s="2" t="s">
@@ -37840,7 +37860,7 @@
       <c r="B48" s="2" t="s">
         <v>1698</v>
       </c>
-      <c r="C48" s="2" t="s">
+      <c r="C48" s="10" t="s">
         <v>1703</v>
       </c>
       <c r="D48" s="2" t="s">
@@ -37863,7 +37883,7 @@
       <c r="B49" s="2" t="s">
         <v>1743</v>
       </c>
-      <c r="C49" s="2" t="s">
+      <c r="C49" s="10" t="s">
         <v>1709</v>
       </c>
       <c r="D49" s="2" t="s">
@@ -37886,7 +37906,7 @@
       <c r="B50" s="2" t="s">
         <v>1731</v>
       </c>
-      <c r="C50" s="2" t="s">
+      <c r="C50" s="10" t="s">
         <v>1710</v>
       </c>
       <c r="D50" s="2" t="s">
@@ -37909,7 +37929,7 @@
       <c r="B51" s="2" t="s">
         <v>1731</v>
       </c>
-      <c r="C51" s="2" t="s">
+      <c r="C51" s="10" t="s">
         <v>1712</v>
       </c>
       <c r="D51" s="2" t="s">
@@ -37932,7 +37952,7 @@
       <c r="B52" s="2" t="s">
         <v>1731</v>
       </c>
-      <c r="C52" s="2" t="s">
+      <c r="C52" s="10" t="s">
         <v>1716</v>
       </c>
       <c r="D52" s="2" t="s">
@@ -37955,7 +37975,7 @@
       <c r="B53" s="2" t="s">
         <v>1731</v>
       </c>
-      <c r="C53" s="2" t="s">
+      <c r="C53" s="10" t="s">
         <v>1717</v>
       </c>
       <c r="D53" s="2" t="s">
@@ -37978,7 +37998,7 @@
       <c r="B54" s="2" t="s">
         <v>1731</v>
       </c>
-      <c r="C54" s="2" t="s">
+      <c r="C54" s="10" t="s">
         <v>1711</v>
       </c>
       <c r="D54" s="2" t="s">
@@ -38001,7 +38021,7 @@
       <c r="B55" s="2" t="s">
         <v>1731</v>
       </c>
-      <c r="C55" s="2" t="s">
+      <c r="C55" s="10" t="s">
         <v>1713</v>
       </c>
       <c r="D55" s="2" t="s">
@@ -38024,7 +38044,7 @@
       <c r="B56" s="2" t="s">
         <v>1731</v>
       </c>
-      <c r="C56" s="2" t="s">
+      <c r="C56" s="10" t="s">
         <v>1718</v>
       </c>
       <c r="D56" s="2" t="s">
@@ -38047,7 +38067,7 @@
       <c r="B57" s="2" t="s">
         <v>1731</v>
       </c>
-      <c r="C57" s="2" t="s">
+      <c r="C57" s="10" t="s">
         <v>1714</v>
       </c>
       <c r="D57" s="2" t="s">
@@ -38070,7 +38090,7 @@
       <c r="B58" s="2" t="s">
         <v>1731</v>
       </c>
-      <c r="C58" s="2" t="s">
+      <c r="C58" s="10" t="s">
         <v>1715</v>
       </c>
       <c r="D58" s="2" t="s">
@@ -38093,7 +38113,7 @@
       <c r="B59" s="2" t="s">
         <v>1755</v>
       </c>
-      <c r="C59" s="2" t="s">
+      <c r="C59" s="10" t="s">
         <v>1719</v>
       </c>
       <c r="D59" s="2" t="s">
@@ -38116,7 +38136,7 @@
       <c r="B60" s="2" t="s">
         <v>1755</v>
       </c>
-      <c r="C60" s="2" t="s">
+      <c r="C60" s="10" t="s">
         <v>1720</v>
       </c>
       <c r="D60" s="2" t="s">
@@ -38139,7 +38159,7 @@
       <c r="B61" s="2" t="s">
         <v>1755</v>
       </c>
-      <c r="C61" s="2" t="s">
+      <c r="C61" s="10" t="s">
         <v>1721</v>
       </c>
       <c r="D61" s="2" t="s">
@@ -38162,7 +38182,7 @@
       <c r="B62" s="2" t="s">
         <v>1755</v>
       </c>
-      <c r="C62" s="2" t="s">
+      <c r="C62" s="10" t="s">
         <v>1722</v>
       </c>
       <c r="D62" s="2" t="s">
@@ -38185,7 +38205,7 @@
       <c r="B63" s="2" t="s">
         <v>1755</v>
       </c>
-      <c r="C63" s="2" t="s">
+      <c r="C63" s="10" t="s">
         <v>1723</v>
       </c>
       <c r="D63" s="2" t="s">
@@ -38208,7 +38228,7 @@
       <c r="B64" s="2" t="s">
         <v>1755</v>
       </c>
-      <c r="C64" s="2" t="s">
+      <c r="C64" s="10" t="s">
         <v>3220</v>
       </c>
       <c r="D64" s="2" t="s">
@@ -38231,7 +38251,7 @@
       <c r="B65" s="2" t="s">
         <v>1755</v>
       </c>
-      <c r="C65" s="2" t="s">
+      <c r="C65" s="10" t="s">
         <v>1724</v>
       </c>
       <c r="D65" s="2" t="s">
@@ -38254,7 +38274,7 @@
       <c r="B66" s="2" t="s">
         <v>1756</v>
       </c>
-      <c r="C66" s="2" t="s">
+      <c r="C66" s="10" t="s">
         <v>1725</v>
       </c>
       <c r="D66" s="2" t="s">
@@ -38277,7 +38297,7 @@
       <c r="B67" s="2" t="s">
         <v>1756</v>
       </c>
-      <c r="C67" s="2" t="s">
+      <c r="C67" s="10" t="s">
         <v>1726</v>
       </c>
       <c r="D67" s="2" t="s">
@@ -38300,7 +38320,7 @@
       <c r="B68" s="2" t="s">
         <v>1756</v>
       </c>
-      <c r="C68" s="2" t="s">
+      <c r="C68" s="10" t="s">
         <v>1728</v>
       </c>
       <c r="D68" s="2" t="s">
@@ -38323,7 +38343,7 @@
       <c r="B69" s="2" t="s">
         <v>1756</v>
       </c>
-      <c r="C69" s="2" t="s">
+      <c r="C69" s="10" t="s">
         <v>1727</v>
       </c>
       <c r="D69" s="2" t="s">
@@ -38346,7 +38366,7 @@
       <c r="B70" s="2" t="s">
         <v>1756</v>
       </c>
-      <c r="C70" s="2" t="s">
+      <c r="C70" s="10" t="s">
         <v>1729</v>
       </c>
       <c r="D70" s="2" t="s">
@@ -38369,7 +38389,7 @@
       <c r="B71" s="2" t="s">
         <v>1756</v>
       </c>
-      <c r="C71" s="2" t="s">
+      <c r="C71" s="10" t="s">
         <v>1730</v>
       </c>
       <c r="D71" s="2" t="s">
@@ -38392,7 +38412,7 @@
       <c r="B72" s="2" t="s">
         <v>1732</v>
       </c>
-      <c r="C72" s="2" t="s">
+      <c r="C72" s="10" t="s">
         <v>1734</v>
       </c>
       <c r="D72" s="2" t="s">
@@ -38415,7 +38435,7 @@
       <c r="B73" s="2" t="s">
         <v>1732</v>
       </c>
-      <c r="C73" s="2" t="s">
+      <c r="C73" s="10" t="s">
         <v>1735</v>
       </c>
       <c r="D73" s="2" t="s">
@@ -38438,7 +38458,7 @@
       <c r="B74" s="2" t="s">
         <v>1732</v>
       </c>
-      <c r="C74" s="2" t="s">
+      <c r="C74" s="10" t="s">
         <v>3221</v>
       </c>
       <c r="D74" s="2" t="s">
@@ -38461,7 +38481,7 @@
       <c r="B75" s="2" t="s">
         <v>1732</v>
       </c>
-      <c r="C75" s="2" t="s">
+      <c r="C75" s="10" t="s">
         <v>1737</v>
       </c>
       <c r="D75" s="2" t="s">
@@ -38484,7 +38504,7 @@
       <c r="B76" s="2" t="s">
         <v>1732</v>
       </c>
-      <c r="C76" s="2" t="s">
+      <c r="C76" s="10" t="s">
         <v>1741</v>
       </c>
       <c r="D76" s="2" t="s">
@@ -38507,7 +38527,7 @@
       <c r="B77" s="2" t="s">
         <v>1732</v>
       </c>
-      <c r="C77" s="2" t="s">
+      <c r="C77" s="10" t="s">
         <v>1738</v>
       </c>
       <c r="D77" s="2" t="s">
@@ -38530,7 +38550,7 @@
       <c r="B78" s="2" t="s">
         <v>1732</v>
       </c>
-      <c r="C78" s="2" t="s">
+      <c r="C78" s="10" t="s">
         <v>1736</v>
       </c>
       <c r="D78" s="2" t="s">
@@ -38553,7 +38573,7 @@
       <c r="B79" s="2" t="s">
         <v>1732</v>
       </c>
-      <c r="C79" s="2" t="s">
+      <c r="C79" s="10" t="s">
         <v>1735</v>
       </c>
       <c r="D79" s="2" t="s">
@@ -38576,7 +38596,7 @@
       <c r="B80" s="2" t="s">
         <v>1732</v>
       </c>
-      <c r="C80" s="2" t="s">
+      <c r="C80" s="10" t="s">
         <v>1740</v>
       </c>
       <c r="D80" s="2" t="s">
@@ -38599,7 +38619,7 @@
       <c r="B81" s="2" t="s">
         <v>3222</v>
       </c>
-      <c r="C81" s="2" t="s">
+      <c r="C81" s="10" t="s">
         <v>3223</v>
       </c>
       <c r="D81" s="2" t="s">
@@ -38622,7 +38642,7 @@
       <c r="B82" s="2" t="s">
         <v>3222</v>
       </c>
-      <c r="C82" s="2" t="s">
+      <c r="C82" s="10" t="s">
         <v>3224</v>
       </c>
       <c r="D82" s="2" t="s">
@@ -38645,7 +38665,7 @@
       <c r="B83" s="2" t="s">
         <v>3222</v>
       </c>
-      <c r="C83" s="2" t="s">
+      <c r="C83" s="10" t="s">
         <v>3225</v>
       </c>
       <c r="D83" s="2" t="s">
@@ -38668,7 +38688,7 @@
       <c r="B84" s="2" t="s">
         <v>3222</v>
       </c>
-      <c r="C84" s="2" t="s">
+      <c r="C84" s="10" t="s">
         <v>3226</v>
       </c>
       <c r="D84" s="2" t="s">
@@ -38691,7 +38711,7 @@
       <c r="B85" s="2" t="s">
         <v>3222</v>
       </c>
-      <c r="C85" s="2" t="s">
+      <c r="C85" s="10" t="s">
         <v>3227</v>
       </c>
       <c r="D85" s="2" t="s">
@@ -38714,7 +38734,7 @@
       <c r="B86" s="2" t="s">
         <v>3222</v>
       </c>
-      <c r="C86" s="2" t="s">
+      <c r="C86" s="10" t="s">
         <v>3228</v>
       </c>
       <c r="D86" s="2" t="s">
@@ -38737,7 +38757,7 @@
       <c r="B87" s="2" t="s">
         <v>3222</v>
       </c>
-      <c r="C87" s="2" t="s">
+      <c r="C87" s="10" t="s">
         <v>3229</v>
       </c>
       <c r="D87" s="2" t="s">
@@ -38760,7 +38780,7 @@
       <c r="B88" s="2" t="s">
         <v>3222</v>
       </c>
-      <c r="C88" s="2" t="s">
+      <c r="C88" s="10" t="s">
         <v>3230</v>
       </c>
       <c r="D88" s="2" t="s">
@@ -38783,7 +38803,7 @@
       <c r="B89" s="2" t="s">
         <v>3222</v>
       </c>
-      <c r="C89" s="2" t="s">
+      <c r="C89" s="10" t="s">
         <v>3231</v>
       </c>
       <c r="D89" s="2" t="s">
@@ -38806,7 +38826,7 @@
       <c r="B90" s="2" t="s">
         <v>1742</v>
       </c>
-      <c r="C90" s="2" t="s">
+      <c r="C90" s="10" t="s">
         <v>1744</v>
       </c>
       <c r="D90" s="2" t="s">
@@ -38829,7 +38849,7 @@
       <c r="B91" s="2" t="s">
         <v>1745</v>
       </c>
-      <c r="C91" s="2" t="s">
+      <c r="C91" s="10" t="s">
         <v>1746</v>
       </c>
       <c r="D91" s="2" t="s">
@@ -38852,7 +38872,7 @@
       <c r="B92" s="2" t="s">
         <v>1745</v>
       </c>
-      <c r="C92" s="2" t="s">
+      <c r="C92" s="10" t="s">
         <v>1747</v>
       </c>
       <c r="D92" s="2" t="s">
@@ -38875,7 +38895,7 @@
       <c r="B93" s="2" t="s">
         <v>1745</v>
       </c>
-      <c r="C93" s="2" t="s">
+      <c r="C93" s="10" t="s">
         <v>1748</v>
       </c>
       <c r="D93" s="2" t="s">
@@ -38898,7 +38918,7 @@
       <c r="B94" s="2" t="s">
         <v>1745</v>
       </c>
-      <c r="C94" s="2" t="s">
+      <c r="C94" s="10" t="s">
         <v>1749</v>
       </c>
       <c r="D94" s="2" t="s">
@@ -38921,7 +38941,7 @@
       <c r="B95" s="2" t="s">
         <v>1745</v>
       </c>
-      <c r="C95" s="2" t="s">
+      <c r="C95" s="10" t="s">
         <v>1750</v>
       </c>
       <c r="D95" s="2" t="s">
@@ -38944,7 +38964,7 @@
       <c r="B96" s="2" t="s">
         <v>1745</v>
       </c>
-      <c r="C96" s="2" t="s">
+      <c r="C96" s="10" t="s">
         <v>1751</v>
       </c>
       <c r="D96" s="2" t="s">
@@ -38967,7 +38987,7 @@
       <c r="B97" s="2" t="s">
         <v>1745</v>
       </c>
-      <c r="C97" s="2" t="s">
+      <c r="C97" s="10" t="s">
         <v>1752</v>
       </c>
       <c r="D97" s="2" t="s">
@@ -38990,7 +39010,7 @@
       <c r="B98" s="2" t="s">
         <v>1745</v>
       </c>
-      <c r="C98" s="2" t="s">
+      <c r="C98" s="10" t="s">
         <v>1753</v>
       </c>
       <c r="D98" s="2" t="s">
@@ -39013,7 +39033,7 @@
       <c r="B99" s="2" t="s">
         <v>1745</v>
       </c>
-      <c r="C99" s="2" t="s">
+      <c r="C99" s="10" t="s">
         <v>1754</v>
       </c>
       <c r="D99" s="2" t="s">
@@ -39036,7 +39056,7 @@
       <c r="B100" s="2" t="s">
         <v>1757</v>
       </c>
-      <c r="C100" s="2" t="s">
+      <c r="C100" s="10" t="s">
         <v>1758</v>
       </c>
       <c r="D100" s="2" t="s">
@@ -39059,7 +39079,7 @@
       <c r="B101" s="2" t="s">
         <v>1757</v>
       </c>
-      <c r="C101" s="2" t="s">
+      <c r="C101" s="10" t="s">
         <v>1759</v>
       </c>
       <c r="D101" s="2" t="s">
@@ -39082,7 +39102,7 @@
       <c r="B102" s="2" t="s">
         <v>1757</v>
       </c>
-      <c r="C102" s="2" t="s">
+      <c r="C102" s="10" t="s">
         <v>1760</v>
       </c>
       <c r="D102" s="2" t="s">
@@ -39105,7 +39125,7 @@
       <c r="B103" s="2" t="s">
         <v>1757</v>
       </c>
-      <c r="C103" s="2" t="s">
+      <c r="C103" s="10" t="s">
         <v>1761</v>
       </c>
       <c r="D103" s="2" t="s">
@@ -39128,7 +39148,7 @@
       <c r="B104" s="2" t="s">
         <v>1757</v>
       </c>
-      <c r="C104" s="2" t="s">
+      <c r="C104" s="10" t="s">
         <v>1762</v>
       </c>
       <c r="D104" s="2" t="s">
@@ -39151,7 +39171,7 @@
       <c r="B105" s="2" t="s">
         <v>1757</v>
       </c>
-      <c r="C105" s="2" t="s">
+      <c r="C105" s="10" t="s">
         <v>3232</v>
       </c>
       <c r="D105" s="2" t="s">
@@ -39174,7 +39194,7 @@
       <c r="B106" s="2" t="s">
         <v>1757</v>
       </c>
-      <c r="C106" s="2" t="s">
+      <c r="C106" s="10" t="s">
         <v>1763</v>
       </c>
       <c r="D106" s="2" t="s">
@@ -39197,7 +39217,7 @@
       <c r="B107" s="2" t="s">
         <v>1733</v>
       </c>
-      <c r="C107" s="2" t="s">
+      <c r="C107" s="10" t="s">
         <v>1764</v>
       </c>
       <c r="D107" s="2" t="s">
@@ -39220,7 +39240,7 @@
       <c r="B108" s="2" t="s">
         <v>1733</v>
       </c>
-      <c r="C108" s="2" t="s">
+      <c r="C108" s="10" t="s">
         <v>1765</v>
       </c>
       <c r="D108" s="2" t="s">
@@ -39243,7 +39263,7 @@
       <c r="B109" s="2" t="s">
         <v>1733</v>
       </c>
-      <c r="C109" s="2" t="s">
+      <c r="C109" s="10" t="s">
         <v>1766</v>
       </c>
       <c r="D109" s="2" t="s">
@@ -39266,7 +39286,7 @@
       <c r="B110" s="2" t="s">
         <v>1733</v>
       </c>
-      <c r="C110" s="2" t="s">
+      <c r="C110" s="10" t="s">
         <v>1767</v>
       </c>
       <c r="D110" s="2" t="s">
@@ -39289,7 +39309,7 @@
       <c r="B111" s="2" t="s">
         <v>1733</v>
       </c>
-      <c r="C111" s="2" t="s">
+      <c r="C111" s="10" t="s">
         <v>1768</v>
       </c>
       <c r="D111" s="2" t="s">
@@ -39312,7 +39332,7 @@
       <c r="B112" s="2" t="s">
         <v>1733</v>
       </c>
-      <c r="C112" s="2" t="s">
+      <c r="C112" s="10" t="s">
         <v>1768</v>
       </c>
       <c r="D112" s="2" t="s">
@@ -39335,7 +39355,7 @@
       <c r="B113" s="2" t="s">
         <v>1733</v>
       </c>
-      <c r="C113" s="2" t="s">
+      <c r="C113" s="10" t="s">
         <v>1770</v>
       </c>
       <c r="D113" s="2" t="s">
@@ -39358,7 +39378,7 @@
       <c r="B114" s="2" t="s">
         <v>1733</v>
       </c>
-      <c r="C114" s="2" t="s">
+      <c r="C114" s="10" t="s">
         <v>1769</v>
       </c>
       <c r="D114" s="2" t="s">
@@ -39381,7 +39401,7 @@
       <c r="B115" s="2" t="s">
         <v>3370</v>
       </c>
-      <c r="C115" s="2" t="s">
+      <c r="C115" s="10" t="s">
         <v>3361</v>
       </c>
       <c r="D115" s="2" t="s">
@@ -39404,7 +39424,7 @@
       <c r="B116" s="2" t="s">
         <v>3370</v>
       </c>
-      <c r="C116" s="2" t="s">
+      <c r="C116" s="10" t="s">
         <v>3362</v>
       </c>
       <c r="D116" s="2" t="s">
@@ -39427,7 +39447,7 @@
       <c r="B117" s="2" t="s">
         <v>3370</v>
       </c>
-      <c r="C117" s="2" t="s">
+      <c r="C117" s="10" t="s">
         <v>3363</v>
       </c>
       <c r="D117" s="2" t="s">
@@ -39450,7 +39470,7 @@
       <c r="B118" s="2" t="s">
         <v>3370</v>
       </c>
-      <c r="C118" s="2" t="s">
+      <c r="C118" s="10" t="s">
         <v>3364</v>
       </c>
       <c r="D118" s="2" t="s">
@@ -39473,7 +39493,7 @@
       <c r="B119" s="2" t="s">
         <v>3370</v>
       </c>
-      <c r="C119" s="2" t="s">
+      <c r="C119" s="10" t="s">
         <v>3365</v>
       </c>
       <c r="D119" s="2" t="s">
@@ -39496,7 +39516,7 @@
       <c r="B120" s="2" t="s">
         <v>3370</v>
       </c>
-      <c r="C120" s="2" t="s">
+      <c r="C120" s="10" t="s">
         <v>3366</v>
       </c>
       <c r="D120" s="2" t="s">
@@ -39519,7 +39539,7 @@
       <c r="B121" s="2" t="s">
         <v>3370</v>
       </c>
-      <c r="C121" s="2" t="s">
+      <c r="C121" s="10" t="s">
         <v>3367</v>
       </c>
       <c r="D121" s="2" t="s">
@@ -39542,7 +39562,7 @@
       <c r="B122" s="2" t="s">
         <v>3370</v>
       </c>
-      <c r="C122" s="2" t="s">
+      <c r="C122" s="10" t="s">
         <v>3368</v>
       </c>
       <c r="D122" s="2" t="s">
@@ -39565,7 +39585,7 @@
       <c r="B123" s="2" t="s">
         <v>3370</v>
       </c>
-      <c r="C123" s="2" t="s">
+      <c r="C123" s="10" t="s">
         <v>3369</v>
       </c>
       <c r="D123" s="2" t="s">
@@ -39588,7 +39608,7 @@
       <c r="B124" s="2" t="s">
         <v>3371</v>
       </c>
-      <c r="C124" s="2" t="s">
+      <c r="C124" s="10" t="s">
         <v>3377</v>
       </c>
       <c r="D124" s="2" t="s">
@@ -39611,7 +39631,7 @@
       <c r="B125" s="2" t="s">
         <v>3371</v>
       </c>
-      <c r="C125" s="2" t="s">
+      <c r="C125" s="10" t="s">
         <v>3378</v>
       </c>
       <c r="D125" s="2" t="s">
@@ -39634,7 +39654,7 @@
       <c r="B126" s="2" t="s">
         <v>3372</v>
       </c>
-      <c r="C126" s="2" t="s">
+      <c r="C126" s="10" t="s">
         <v>3375</v>
       </c>
       <c r="D126" s="2" t="s">
@@ -39657,7 +39677,7 @@
       <c r="B127" s="2" t="s">
         <v>3372</v>
       </c>
-      <c r="C127" s="2" t="s">
+      <c r="C127" s="10" t="s">
         <v>3376</v>
       </c>
       <c r="D127" s="2" t="s">
@@ -39680,7 +39700,7 @@
       <c r="B128" s="2" t="s">
         <v>3373</v>
       </c>
-      <c r="C128" s="2" t="s">
+      <c r="C128" s="10" t="s">
         <v>3380</v>
       </c>
       <c r="D128" s="2" t="s">
@@ -39703,7 +39723,7 @@
       <c r="B129" s="2" t="s">
         <v>3373</v>
       </c>
-      <c r="C129" s="2" t="s">
+      <c r="C129" s="10" t="s">
         <v>3379</v>
       </c>
       <c r="D129" s="2" t="s">
@@ -39726,7 +39746,7 @@
       <c r="B130" s="2" t="s">
         <v>3374</v>
       </c>
-      <c r="C130" s="2" t="s">
+      <c r="C130" s="10" t="s">
         <v>3381</v>
       </c>
       <c r="D130" s="2" t="s">
@@ -39749,7 +39769,7 @@
       <c r="B131" s="2" t="s">
         <v>3374</v>
       </c>
-      <c r="C131" s="2" t="s">
+      <c r="C131" s="10" t="s">
         <v>3382</v>
       </c>
       <c r="D131" s="2" t="s">
@@ -39772,7 +39792,7 @@
       <c r="B132" s="2" t="s">
         <v>3255</v>
       </c>
-      <c r="C132" s="2" t="s">
+      <c r="C132" s="10" t="s">
         <v>3244</v>
       </c>
       <c r="D132" s="2" t="s">
@@ -39795,7 +39815,7 @@
       <c r="B133" s="2" t="s">
         <v>3242</v>
       </c>
-      <c r="C133" s="2" t="s">
+      <c r="C133" s="10" t="s">
         <v>3245</v>
       </c>
       <c r="D133" s="2" t="s">
@@ -39818,7 +39838,7 @@
       <c r="B134" s="2" t="s">
         <v>3243</v>
       </c>
-      <c r="C134" s="2" t="s">
+      <c r="C134" s="10" t="s">
         <v>3246</v>
       </c>
       <c r="D134" s="2" t="s">
@@ -39841,7 +39861,7 @@
       <c r="B135" s="2" t="s">
         <v>3243</v>
       </c>
-      <c r="C135" s="2" t="s">
+      <c r="C135" s="10" t="s">
         <v>3247</v>
       </c>
       <c r="D135" s="2" t="s">
@@ -39864,7 +39884,7 @@
       <c r="B136" s="2" t="s">
         <v>3243</v>
       </c>
-      <c r="C136" s="2" t="s">
+      <c r="C136" s="10" t="s">
         <v>3248</v>
       </c>
       <c r="D136" s="2" t="s">
@@ -39887,7 +39907,7 @@
       <c r="B137" s="2" t="s">
         <v>3243</v>
       </c>
-      <c r="C137" s="2" t="s">
+      <c r="C137" s="10" t="s">
         <v>3249</v>
       </c>
       <c r="D137" s="2" t="s">
@@ -39910,7 +39930,7 @@
       <c r="B138" s="2" t="s">
         <v>3243</v>
       </c>
-      <c r="C138" s="2" t="s">
+      <c r="C138" s="10" t="s">
         <v>3250</v>
       </c>
       <c r="D138" s="2" t="s">
@@ -39933,7 +39953,7 @@
       <c r="B139" s="2" t="s">
         <v>3243</v>
       </c>
-      <c r="C139" s="2" t="s">
+      <c r="C139" s="10" t="s">
         <v>3251</v>
       </c>
       <c r="D139" s="2" t="s">
@@ -39956,7 +39976,7 @@
       <c r="B140" s="2" t="s">
         <v>3243</v>
       </c>
-      <c r="C140" s="2" t="s">
+      <c r="C140" s="10" t="s">
         <v>3252</v>
       </c>
       <c r="D140" s="2" t="s">
@@ -39979,7 +39999,7 @@
       <c r="B141" s="2" t="s">
         <v>3243</v>
       </c>
-      <c r="C141" s="2" t="s">
+      <c r="C141" s="10" t="s">
         <v>3253</v>
       </c>
       <c r="D141" s="2" t="s">
@@ -40002,7 +40022,7 @@
       <c r="B142" s="2" t="s">
         <v>3243</v>
       </c>
-      <c r="C142" s="2" t="s">
+      <c r="C142" s="10" t="s">
         <v>3254</v>
       </c>
       <c r="D142" s="2" t="s">
@@ -40025,7 +40045,7 @@
       <c r="B143" s="2" t="s">
         <v>3256</v>
       </c>
-      <c r="C143" s="2" t="s">
+      <c r="C143" s="10" t="s">
         <v>3286</v>
       </c>
       <c r="D143" s="2" t="s">
@@ -40048,7 +40068,7 @@
       <c r="B144" s="2" t="s">
         <v>3256</v>
       </c>
-      <c r="C144" s="2" t="s">
+      <c r="C144" s="10" t="s">
         <v>3258</v>
       </c>
       <c r="D144" s="2" t="s">
@@ -40071,7 +40091,7 @@
       <c r="B145" s="2" t="s">
         <v>3256</v>
       </c>
-      <c r="C145" s="2" t="s">
+      <c r="C145" s="10" t="s">
         <v>3259</v>
       </c>
       <c r="D145" s="2" t="s">
@@ -40094,7 +40114,7 @@
       <c r="B146" s="2" t="s">
         <v>3256</v>
       </c>
-      <c r="C146" s="2" t="s">
+      <c r="C146" s="10" t="s">
         <v>3260</v>
       </c>
       <c r="D146" s="2" t="s">
@@ -40117,7 +40137,7 @@
       <c r="B147" s="2" t="s">
         <v>3256</v>
       </c>
-      <c r="C147" s="2" t="s">
+      <c r="C147" s="10" t="s">
         <v>3261</v>
       </c>
       <c r="D147" s="2" t="s">
@@ -40140,7 +40160,7 @@
       <c r="B148" s="2" t="s">
         <v>3256</v>
       </c>
-      <c r="C148" s="2" t="s">
+      <c r="C148" s="10" t="s">
         <v>3262</v>
       </c>
       <c r="D148" s="2" t="s">
@@ -40163,7 +40183,7 @@
       <c r="B149" s="2" t="s">
         <v>3256</v>
       </c>
-      <c r="C149" s="2" t="s">
+      <c r="C149" s="10" t="s">
         <v>3263</v>
       </c>
       <c r="D149" s="2" t="s">
@@ -40186,7 +40206,7 @@
       <c r="B150" s="2" t="s">
         <v>3257</v>
       </c>
-      <c r="C150" s="2" t="s">
+      <c r="C150" s="10" t="s">
         <v>3264</v>
       </c>
       <c r="D150" s="2" t="s">
@@ -40209,7 +40229,7 @@
       <c r="B151" s="2" t="s">
         <v>3257</v>
       </c>
-      <c r="C151" s="2" t="s">
+      <c r="C151" s="10" t="s">
         <v>3265</v>
       </c>
       <c r="D151" s="2" t="s">
@@ -40232,7 +40252,7 @@
       <c r="B152" s="2" t="s">
         <v>3257</v>
       </c>
-      <c r="C152" s="2" t="s">
+      <c r="C152" s="10" t="s">
         <v>3266</v>
       </c>
       <c r="D152" s="2" t="s">
@@ -40255,7 +40275,7 @@
       <c r="B153" s="2" t="s">
         <v>3257</v>
       </c>
-      <c r="C153" s="2" t="s">
+      <c r="C153" s="10" t="s">
         <v>3267</v>
       </c>
       <c r="D153" s="2" t="s">
@@ -40278,7 +40298,7 @@
       <c r="B154" s="2" t="s">
         <v>3257</v>
       </c>
-      <c r="C154" s="2" t="s">
+      <c r="C154" s="10" t="s">
         <v>3268</v>
       </c>
       <c r="D154" s="2" t="s">
@@ -40301,7 +40321,7 @@
       <c r="B155" s="2" t="s">
         <v>3257</v>
       </c>
-      <c r="C155" s="2" t="s">
+      <c r="C155" s="10" t="s">
         <v>3268</v>
       </c>
       <c r="D155" s="2" t="s">
@@ -40324,7 +40344,7 @@
       <c r="B156" s="2" t="s">
         <v>3257</v>
       </c>
-      <c r="C156" s="2" t="s">
+      <c r="C156" s="10" t="s">
         <v>3269</v>
       </c>
       <c r="D156" s="2" t="s">
@@ -40347,7 +40367,7 @@
       <c r="B157" s="2" t="s">
         <v>3257</v>
       </c>
-      <c r="C157" s="2" t="s">
+      <c r="C157" s="10" t="s">
         <v>3270</v>
       </c>
       <c r="D157" s="2" t="s">
@@ -40370,7 +40390,7 @@
       <c r="B158" s="2" t="s">
         <v>3271</v>
       </c>
-      <c r="C158" s="2" t="s">
+      <c r="C158" s="10" t="s">
         <v>3244</v>
       </c>
       <c r="D158" s="2" t="s">
@@ -40393,7 +40413,7 @@
       <c r="B159" s="2" t="s">
         <v>3272</v>
       </c>
-      <c r="C159" s="2" t="s">
+      <c r="C159" s="10" t="s">
         <v>3276</v>
       </c>
       <c r="D159" s="2" t="s">
@@ -40416,7 +40436,7 @@
       <c r="B160" s="2" t="s">
         <v>3273</v>
       </c>
-      <c r="C160" s="2" t="s">
+      <c r="C160" s="10" t="s">
         <v>3277</v>
       </c>
       <c r="D160" s="2" t="s">
@@ -40439,7 +40459,7 @@
       <c r="B161" s="2" t="s">
         <v>3273</v>
       </c>
-      <c r="C161" s="2" t="s">
+      <c r="C161" s="10" t="s">
         <v>3278</v>
       </c>
       <c r="D161" s="2" t="s">
@@ -40462,7 +40482,7 @@
       <c r="B162" s="2" t="s">
         <v>3273</v>
       </c>
-      <c r="C162" s="2" t="s">
+      <c r="C162" s="10" t="s">
         <v>3279</v>
       </c>
       <c r="D162" s="2" t="s">
@@ -40485,7 +40505,7 @@
       <c r="B163" s="2" t="s">
         <v>3273</v>
       </c>
-      <c r="C163" s="2" t="s">
+      <c r="C163" s="10" t="s">
         <v>3280</v>
       </c>
       <c r="D163" s="2" t="s">
@@ -40508,7 +40528,7 @@
       <c r="B164" s="2" t="s">
         <v>3273</v>
       </c>
-      <c r="C164" s="2" t="s">
+      <c r="C164" s="10" t="s">
         <v>3281</v>
       </c>
       <c r="D164" s="2" t="s">
@@ -40531,7 +40551,7 @@
       <c r="B165" s="2" t="s">
         <v>3273</v>
       </c>
-      <c r="C165" s="2" t="s">
+      <c r="C165" s="10" t="s">
         <v>3282</v>
       </c>
       <c r="D165" s="2" t="s">
@@ -40554,7 +40574,7 @@
       <c r="B166" s="2" t="s">
         <v>3273</v>
       </c>
-      <c r="C166" s="2" t="s">
+      <c r="C166" s="10" t="s">
         <v>3283</v>
       </c>
       <c r="D166" s="2" t="s">
@@ -40577,7 +40597,7 @@
       <c r="B167" s="2" t="s">
         <v>3273</v>
       </c>
-      <c r="C167" s="2" t="s">
+      <c r="C167" s="10" t="s">
         <v>3284</v>
       </c>
       <c r="D167" s="2" t="s">
@@ -40600,7 +40620,7 @@
       <c r="B168" s="2" t="s">
         <v>3273</v>
       </c>
-      <c r="C168" s="2" t="s">
+      <c r="C168" s="10" t="s">
         <v>3285</v>
       </c>
       <c r="D168" s="2" t="s">
@@ -40623,7 +40643,7 @@
       <c r="B169" s="2" t="s">
         <v>3274</v>
       </c>
-      <c r="C169" s="2" t="s">
+      <c r="C169" s="10" t="s">
         <v>3287</v>
       </c>
       <c r="D169" s="2" t="s">
@@ -40646,7 +40666,7 @@
       <c r="B170" s="2" t="s">
         <v>3274</v>
       </c>
-      <c r="C170" s="2" t="s">
+      <c r="C170" s="10" t="s">
         <v>3288</v>
       </c>
       <c r="D170" s="2" t="s">
@@ -40669,7 +40689,7 @@
       <c r="B171" s="2" t="s">
         <v>3274</v>
       </c>
-      <c r="C171" s="2" t="s">
+      <c r="C171" s="10" t="s">
         <v>3289</v>
       </c>
       <c r="D171" s="2" t="s">
@@ -40692,7 +40712,7 @@
       <c r="B172" s="2" t="s">
         <v>3274</v>
       </c>
-      <c r="C172" s="2" t="s">
+      <c r="C172" s="10" t="s">
         <v>3290</v>
       </c>
       <c r="D172" s="2" t="s">
@@ -40715,7 +40735,7 @@
       <c r="B173" s="2" t="s">
         <v>3274</v>
       </c>
-      <c r="C173" s="2" t="s">
+      <c r="C173" s="10" t="s">
         <v>3291</v>
       </c>
       <c r="D173" s="2" t="s">
@@ -40738,7 +40758,7 @@
       <c r="B174" s="2" t="s">
         <v>3274</v>
       </c>
-      <c r="C174" s="2" t="s">
+      <c r="C174" s="10" t="s">
         <v>3292</v>
       </c>
       <c r="D174" s="2" t="s">
@@ -40761,7 +40781,7 @@
       <c r="B175" s="2" t="s">
         <v>3274</v>
       </c>
-      <c r="C175" s="2" t="s">
+      <c r="C175" s="10" t="s">
         <v>3293</v>
       </c>
       <c r="D175" s="2" t="s">
@@ -40784,7 +40804,7 @@
       <c r="B176" s="2" t="s">
         <v>3275</v>
       </c>
-      <c r="C176" s="2" t="s">
+      <c r="C176" s="10" t="s">
         <v>3294</v>
       </c>
       <c r="D176" s="2" t="s">
@@ -40807,7 +40827,7 @@
       <c r="B177" s="2" t="s">
         <v>3275</v>
       </c>
-      <c r="C177" s="2" t="s">
+      <c r="C177" s="10" t="s">
         <v>3295</v>
       </c>
       <c r="D177" s="2" t="s">
@@ -40830,7 +40850,7 @@
       <c r="B178" s="2" t="s">
         <v>3275</v>
       </c>
-      <c r="C178" s="2" t="s">
+      <c r="C178" s="10" t="s">
         <v>3296</v>
       </c>
       <c r="D178" s="2" t="s">
@@ -40853,7 +40873,7 @@
       <c r="B179" s="2" t="s">
         <v>3275</v>
       </c>
-      <c r="C179" s="2" t="s">
+      <c r="C179" s="10" t="s">
         <v>3297</v>
       </c>
       <c r="D179" s="2" t="s">
@@ -40876,7 +40896,7 @@
       <c r="B180" s="2" t="s">
         <v>3275</v>
       </c>
-      <c r="C180" s="2" t="s">
+      <c r="C180" s="10" t="s">
         <v>3298</v>
       </c>
       <c r="D180" s="2" t="s">
@@ -40899,7 +40919,7 @@
       <c r="B181" s="2" t="s">
         <v>3275</v>
       </c>
-      <c r="C181" s="2" t="s">
+      <c r="C181" s="10" t="s">
         <v>3298</v>
       </c>
       <c r="D181" s="2" t="s">
@@ -40922,7 +40942,7 @@
       <c r="B182" s="2" t="s">
         <v>3275</v>
       </c>
-      <c r="C182" s="2" t="s">
+      <c r="C182" s="10" t="s">
         <v>3299</v>
       </c>
       <c r="D182" s="2" t="s">
@@ -40945,7 +40965,7 @@
       <c r="B183" s="2" t="s">
         <v>3275</v>
       </c>
-      <c r="C183" s="2" t="s">
+      <c r="C183" s="10" t="s">
         <v>3300</v>
       </c>
       <c r="D183" s="2" t="s">
@@ -40968,7 +40988,7 @@
       <c r="B184" s="2" t="s">
         <v>3301</v>
       </c>
-      <c r="C184" s="2" t="s">
+      <c r="C184" s="10" t="s">
         <v>3306</v>
       </c>
       <c r="D184" s="2" t="s">
@@ -40991,7 +41011,7 @@
       <c r="B185" s="2" t="s">
         <v>3302</v>
       </c>
-      <c r="C185" s="2" t="s">
+      <c r="C185" s="10" t="s">
         <v>3307</v>
       </c>
       <c r="D185" s="2" t="s">
@@ -41014,7 +41034,7 @@
       <c r="B186" s="2" t="s">
         <v>3303</v>
       </c>
-      <c r="C186" s="2" t="s">
+      <c r="C186" s="10" t="s">
         <v>3308</v>
       </c>
       <c r="D186" s="2" t="s">
@@ -41037,7 +41057,7 @@
       <c r="B187" s="2" t="s">
         <v>3303</v>
       </c>
-      <c r="C187" s="2" t="s">
+      <c r="C187" s="10" t="s">
         <v>3309</v>
       </c>
       <c r="D187" s="2" t="s">
@@ -41060,7 +41080,7 @@
       <c r="B188" s="2" t="s">
         <v>3303</v>
       </c>
-      <c r="C188" s="2" t="s">
+      <c r="C188" s="10" t="s">
         <v>3310</v>
       </c>
       <c r="D188" s="2" t="s">
@@ -41083,7 +41103,7 @@
       <c r="B189" s="2" t="s">
         <v>3303</v>
       </c>
-      <c r="C189" s="2" t="s">
+      <c r="C189" s="10" t="s">
         <v>3311</v>
       </c>
       <c r="D189" s="2" t="s">
@@ -41106,7 +41126,7 @@
       <c r="B190" s="2" t="s">
         <v>3303</v>
       </c>
-      <c r="C190" s="2" t="s">
+      <c r="C190" s="10" t="s">
         <v>3312</v>
       </c>
       <c r="D190" s="2" t="s">
@@ -41129,7 +41149,7 @@
       <c r="B191" s="2" t="s">
         <v>3303</v>
       </c>
-      <c r="C191" s="2" t="s">
+      <c r="C191" s="10" t="s">
         <v>3313</v>
       </c>
       <c r="D191" s="2" t="s">
@@ -41152,7 +41172,7 @@
       <c r="B192" s="2" t="s">
         <v>3303</v>
       </c>
-      <c r="C192" s="2" t="s">
+      <c r="C192" s="10" t="s">
         <v>3314</v>
       </c>
       <c r="D192" s="2" t="s">
@@ -41175,7 +41195,7 @@
       <c r="B193" s="2" t="s">
         <v>3303</v>
       </c>
-      <c r="C193" s="2" t="s">
+      <c r="C193" s="10" t="s">
         <v>3315</v>
       </c>
       <c r="D193" s="2" t="s">
@@ -41198,7 +41218,7 @@
       <c r="B194" s="2" t="s">
         <v>3303</v>
       </c>
-      <c r="C194" s="2" t="s">
+      <c r="C194" s="10" t="s">
         <v>3316</v>
       </c>
       <c r="D194" s="2" t="s">
@@ -41221,7 +41241,7 @@
       <c r="B195" s="2" t="s">
         <v>3304</v>
       </c>
-      <c r="C195" s="2" t="s">
+      <c r="C195" s="10" t="s">
         <v>3317</v>
       </c>
       <c r="D195" s="2" t="s">
@@ -41244,7 +41264,7 @@
       <c r="B196" s="2" t="s">
         <v>3304</v>
       </c>
-      <c r="C196" s="2" t="s">
+      <c r="C196" s="10" t="s">
         <v>3318</v>
       </c>
       <c r="D196" s="2" t="s">
@@ -41267,7 +41287,7 @@
       <c r="B197" s="2" t="s">
         <v>3304</v>
       </c>
-      <c r="C197" s="2" t="s">
+      <c r="C197" s="10" t="s">
         <v>3319</v>
       </c>
       <c r="D197" s="2" t="s">
@@ -41290,7 +41310,7 @@
       <c r="B198" s="2" t="s">
         <v>3304</v>
       </c>
-      <c r="C198" s="2" t="s">
+      <c r="C198" s="10" t="s">
         <v>3320</v>
       </c>
       <c r="D198" s="2" t="s">
@@ -41313,7 +41333,7 @@
       <c r="B199" s="2" t="s">
         <v>3304</v>
       </c>
-      <c r="C199" s="2" t="s">
+      <c r="C199" s="10" t="s">
         <v>3321</v>
       </c>
       <c r="D199" s="2" t="s">
@@ -41336,7 +41356,7 @@
       <c r="B200" s="2" t="s">
         <v>3304</v>
       </c>
-      <c r="C200" s="2" t="s">
+      <c r="C200" s="10" t="s">
         <v>3322</v>
       </c>
       <c r="D200" s="2" t="s">
@@ -41359,7 +41379,7 @@
       <c r="B201" s="2" t="s">
         <v>3304</v>
       </c>
-      <c r="C201" s="2" t="s">
+      <c r="C201" s="10" t="s">
         <v>3323</v>
       </c>
       <c r="D201" s="2" t="s">
@@ -41382,7 +41402,7 @@
       <c r="B202" s="2" t="s">
         <v>3305</v>
       </c>
-      <c r="C202" s="2" t="s">
+      <c r="C202" s="10" t="s">
         <v>3324</v>
       </c>
       <c r="D202" s="2" t="s">
@@ -41405,7 +41425,7 @@
       <c r="B203" s="2" t="s">
         <v>3305</v>
       </c>
-      <c r="C203" s="2" t="s">
+      <c r="C203" s="10" t="s">
         <v>3325</v>
       </c>
       <c r="D203" s="2" t="s">
@@ -41428,7 +41448,7 @@
       <c r="B204" s="2" t="s">
         <v>3305</v>
       </c>
-      <c r="C204" s="2" t="s">
+      <c r="C204" s="10" t="s">
         <v>3326</v>
       </c>
       <c r="D204" s="2" t="s">
@@ -41451,7 +41471,7 @@
       <c r="B205" s="2" t="s">
         <v>3305</v>
       </c>
-      <c r="C205" s="2" t="s">
+      <c r="C205" s="10" t="s">
         <v>3327</v>
       </c>
       <c r="D205" s="2" t="s">
@@ -41474,7 +41494,7 @@
       <c r="B206" s="2" t="s">
         <v>3305</v>
       </c>
-      <c r="C206" s="2" t="s">
+      <c r="C206" s="10" t="s">
         <v>3328</v>
       </c>
       <c r="D206" s="2" t="s">
@@ -41497,7 +41517,7 @@
       <c r="B207" s="2" t="s">
         <v>3305</v>
       </c>
-      <c r="C207" s="2" t="s">
+      <c r="C207" s="10" t="s">
         <v>3328</v>
       </c>
       <c r="D207" s="2" t="s">
@@ -41520,7 +41540,7 @@
       <c r="B208" s="2" t="s">
         <v>3305</v>
       </c>
-      <c r="C208" s="2" t="s">
+      <c r="C208" s="10" t="s">
         <v>3329</v>
       </c>
       <c r="D208" s="2" t="s">
@@ -41543,7 +41563,7 @@
       <c r="B209" s="2" t="s">
         <v>3305</v>
       </c>
-      <c r="C209" s="2" t="s">
+      <c r="C209" s="10" t="s">
         <v>3330</v>
       </c>
       <c r="D209" s="2" t="s">
@@ -41566,7 +41586,7 @@
       <c r="B210" s="2" t="s">
         <v>3331</v>
       </c>
-      <c r="C210" s="2" t="s">
+      <c r="C210" s="10" t="s">
         <v>3332</v>
       </c>
       <c r="D210" s="2" t="s">
@@ -41589,7 +41609,7 @@
       <c r="B211" s="2" t="s">
         <v>3333</v>
       </c>
-      <c r="C211" s="2" t="s">
+      <c r="C211" s="10" t="s">
         <v>3337</v>
       </c>
       <c r="D211" s="2" t="s">
@@ -41612,7 +41632,7 @@
       <c r="B212" s="2" t="s">
         <v>3334</v>
       </c>
-      <c r="C212" s="2" t="s">
+      <c r="C212" s="10" t="s">
         <v>3338</v>
       </c>
       <c r="D212" s="2" t="s">
@@ -41635,7 +41655,7 @@
       <c r="B213" s="2" t="s">
         <v>3334</v>
       </c>
-      <c r="C213" s="2" t="s">
+      <c r="C213" s="10" t="s">
         <v>3339</v>
       </c>
       <c r="D213" s="2" t="s">
@@ -41658,7 +41678,7 @@
       <c r="B214" s="2" t="s">
         <v>3334</v>
       </c>
-      <c r="C214" s="2" t="s">
+      <c r="C214" s="10" t="s">
         <v>3340</v>
       </c>
       <c r="D214" s="2" t="s">
@@ -41681,7 +41701,7 @@
       <c r="B215" s="2" t="s">
         <v>3334</v>
       </c>
-      <c r="C215" s="2" t="s">
+      <c r="C215" s="10" t="s">
         <v>3341</v>
       </c>
       <c r="D215" s="2" t="s">
@@ -41704,7 +41724,7 @@
       <c r="B216" s="2" t="s">
         <v>3334</v>
       </c>
-      <c r="C216" s="2" t="s">
+      <c r="C216" s="10" t="s">
         <v>3342</v>
       </c>
       <c r="D216" s="2" t="s">
@@ -41727,7 +41747,7 @@
       <c r="B217" s="2" t="s">
         <v>3334</v>
       </c>
-      <c r="C217" s="2" t="s">
+      <c r="C217" s="10" t="s">
         <v>3343</v>
       </c>
       <c r="D217" s="2" t="s">
@@ -41750,7 +41770,7 @@
       <c r="B218" s="2" t="s">
         <v>3334</v>
       </c>
-      <c r="C218" s="2" t="s">
+      <c r="C218" s="10" t="s">
         <v>3344</v>
       </c>
       <c r="D218" s="2" t="s">
@@ -41773,7 +41793,7 @@
       <c r="B219" s="2" t="s">
         <v>3334</v>
       </c>
-      <c r="C219" s="2" t="s">
+      <c r="C219" s="10" t="s">
         <v>3345</v>
       </c>
       <c r="D219" s="2" t="s">
@@ -41796,7 +41816,7 @@
       <c r="B220" s="2" t="s">
         <v>3334</v>
       </c>
-      <c r="C220" s="2" t="s">
+      <c r="C220" s="10" t="s">
         <v>3346</v>
       </c>
       <c r="D220" s="2" t="s">
@@ -41819,7 +41839,7 @@
       <c r="B221" s="2" t="s">
         <v>3335</v>
       </c>
-      <c r="C221" s="2" t="s">
+      <c r="C221" s="10" t="s">
         <v>3347</v>
       </c>
       <c r="D221" s="2" t="s">
@@ -41842,7 +41862,7 @@
       <c r="B222" s="2" t="s">
         <v>3335</v>
       </c>
-      <c r="C222" s="2" t="s">
+      <c r="C222" s="10" t="s">
         <v>3348</v>
       </c>
       <c r="D222" s="2" t="s">
@@ -41865,7 +41885,7 @@
       <c r="B223" s="2" t="s">
         <v>3335</v>
       </c>
-      <c r="C223" s="2" t="s">
+      <c r="C223" s="10" t="s">
         <v>3349</v>
       </c>
       <c r="D223" s="2" t="s">
@@ -41888,7 +41908,7 @@
       <c r="B224" s="2" t="s">
         <v>3335</v>
       </c>
-      <c r="C224" s="2" t="s">
+      <c r="C224" s="10" t="s">
         <v>3350</v>
       </c>
       <c r="D224" s="2" t="s">
@@ -41911,7 +41931,7 @@
       <c r="B225" s="2" t="s">
         <v>3335</v>
       </c>
-      <c r="C225" s="2" t="s">
+      <c r="C225" s="10" t="s">
         <v>3351</v>
       </c>
       <c r="D225" s="2" t="s">
@@ -41934,7 +41954,7 @@
       <c r="B226" s="2" t="s">
         <v>3335</v>
       </c>
-      <c r="C226" s="2" t="s">
+      <c r="C226" s="10" t="s">
         <v>3352</v>
       </c>
       <c r="D226" s="2" t="s">
@@ -41957,7 +41977,7 @@
       <c r="B227" s="2" t="s">
         <v>3335</v>
       </c>
-      <c r="C227" s="2" t="s">
+      <c r="C227" s="10" t="s">
         <v>3353</v>
       </c>
       <c r="D227" s="2" t="s">
@@ -41980,7 +42000,7 @@
       <c r="B228" s="2" t="s">
         <v>3336</v>
       </c>
-      <c r="C228" s="2" t="s">
+      <c r="C228" s="10" t="s">
         <v>3354</v>
       </c>
       <c r="D228" s="2" t="s">
@@ -42003,7 +42023,7 @@
       <c r="B229" s="2" t="s">
         <v>3336</v>
       </c>
-      <c r="C229" s="2" t="s">
+      <c r="C229" s="10" t="s">
         <v>3355</v>
       </c>
       <c r="D229" s="2" t="s">
@@ -42026,7 +42046,7 @@
       <c r="B230" s="2" t="s">
         <v>3336</v>
       </c>
-      <c r="C230" s="2" t="s">
+      <c r="C230" s="10" t="s">
         <v>3356</v>
       </c>
       <c r="D230" s="2" t="s">
@@ -42049,7 +42069,7 @@
       <c r="B231" s="2" t="s">
         <v>3336</v>
       </c>
-      <c r="C231" s="2" t="s">
+      <c r="C231" s="10" t="s">
         <v>3357</v>
       </c>
       <c r="D231" s="2" t="s">
@@ -42072,7 +42092,7 @@
       <c r="B232" s="2" t="s">
         <v>3336</v>
       </c>
-      <c r="C232" s="2" t="s">
+      <c r="C232" s="10" t="s">
         <v>3358</v>
       </c>
       <c r="D232" s="2" t="s">
@@ -42095,7 +42115,7 @@
       <c r="B233" s="2" t="s">
         <v>3336</v>
       </c>
-      <c r="C233" s="2" t="s">
+      <c r="C233" s="10" t="s">
         <v>3358</v>
       </c>
       <c r="D233" s="2" t="s">
@@ -42118,7 +42138,7 @@
       <c r="B234" s="2" t="s">
         <v>3336</v>
       </c>
-      <c r="C234" s="2" t="s">
+      <c r="C234" s="10" t="s">
         <v>3359</v>
       </c>
       <c r="D234" s="2" t="s">
@@ -42141,7 +42161,7 @@
       <c r="B235" s="2" t="s">
         <v>3336</v>
       </c>
-      <c r="C235" s="2" t="s">
+      <c r="C235" s="10" t="s">
         <v>3360</v>
       </c>
       <c r="D235" s="2" t="s">
@@ -42164,7 +42184,7 @@
       <c r="B236" s="2" t="s">
         <v>3395</v>
       </c>
-      <c r="C236" s="2" t="s">
+      <c r="C236" s="10" t="s">
         <v>3233</v>
       </c>
       <c r="D236" s="2" t="s">
@@ -42187,7 +42207,7 @@
       <c r="B237" s="2" t="s">
         <v>3395</v>
       </c>
-      <c r="C237" s="2" t="s">
+      <c r="C237" s="10" t="s">
         <v>3234</v>
       </c>
       <c r="D237" s="2" t="s">
@@ -42210,7 +42230,7 @@
       <c r="B238" s="2" t="s">
         <v>3395</v>
       </c>
-      <c r="C238" s="2" t="s">
+      <c r="C238" s="10" t="s">
         <v>3235</v>
       </c>
       <c r="D238" s="2" t="s">
@@ -42233,7 +42253,7 @@
       <c r="B239" s="2" t="s">
         <v>3395</v>
       </c>
-      <c r="C239" s="2" t="s">
+      <c r="C239" s="10" t="s">
         <v>3236</v>
       </c>
       <c r="D239" s="2" t="s">
@@ -42256,7 +42276,7 @@
       <c r="B240" s="2" t="s">
         <v>3395</v>
       </c>
-      <c r="C240" s="2" t="s">
+      <c r="C240" s="10" t="s">
         <v>3237</v>
       </c>
       <c r="D240" s="2" t="s">
@@ -42279,7 +42299,7 @@
       <c r="B241" s="2" t="s">
         <v>3395</v>
       </c>
-      <c r="C241" s="2" t="s">
+      <c r="C241" s="10" t="s">
         <v>3238</v>
       </c>
       <c r="D241" s="2" t="s">
@@ -42302,7 +42322,7 @@
       <c r="B242" s="2" t="s">
         <v>3395</v>
       </c>
-      <c r="C242" s="2" t="s">
+      <c r="C242" s="10" t="s">
         <v>3239</v>
       </c>
       <c r="D242" s="2" t="s">
@@ -42325,7 +42345,7 @@
       <c r="B243" s="2" t="s">
         <v>3395</v>
       </c>
-      <c r="C243" s="2" t="s">
+      <c r="C243" s="10" t="s">
         <v>3240</v>
       </c>
       <c r="D243" s="2" t="s">
@@ -42348,7 +42368,7 @@
       <c r="B244" s="2" t="s">
         <v>3395</v>
       </c>
-      <c r="C244" s="2" t="s">
+      <c r="C244" s="10" t="s">
         <v>3241</v>
       </c>
       <c r="D244" s="2" t="s">
@@ -42371,7 +42391,7 @@
       <c r="B245" s="2" t="s">
         <v>3396</v>
       </c>
-      <c r="C245" s="2" t="s">
+      <c r="C245" s="10" t="s">
         <v>3383</v>
       </c>
       <c r="D245" s="2" t="s">
@@ -42394,7 +42414,7 @@
       <c r="B246" s="2" t="s">
         <v>3396</v>
       </c>
-      <c r="C246" s="2" t="s">
+      <c r="C246" s="10" t="s">
         <v>3387</v>
       </c>
       <c r="D246" s="2" t="s">
@@ -42417,7 +42437,7 @@
       <c r="B247" s="2" t="s">
         <v>3396</v>
       </c>
-      <c r="C247" s="2" t="s">
+      <c r="C247" s="10" t="s">
         <v>3384</v>
       </c>
       <c r="D247" s="2" t="s">
@@ -42440,7 +42460,7 @@
       <c r="B248" s="2" t="s">
         <v>3396</v>
       </c>
-      <c r="C248" s="2" t="s">
+      <c r="C248" s="10" t="s">
         <v>3385</v>
       </c>
       <c r="D248" s="2" t="s">
@@ -42463,7 +42483,7 @@
       <c r="B249" s="2" t="s">
         <v>3396</v>
       </c>
-      <c r="C249" s="2" t="s">
+      <c r="C249" s="10" t="s">
         <v>3386</v>
       </c>
       <c r="D249" s="2" t="s">
@@ -42486,7 +42506,7 @@
       <c r="B250" s="2" t="s">
         <v>3393</v>
       </c>
-      <c r="C250" s="2" t="s">
+      <c r="C250" s="10" t="s">
         <v>3388</v>
       </c>
       <c r="D250" s="2" t="s">
@@ -42509,7 +42529,7 @@
       <c r="B251" s="2" t="s">
         <v>3393</v>
       </c>
-      <c r="C251" s="2" t="s">
+      <c r="C251" s="10" t="s">
         <v>3389</v>
       </c>
       <c r="D251" s="2" t="s">
@@ -42532,7 +42552,7 @@
       <c r="B252" s="2" t="s">
         <v>3393</v>
       </c>
-      <c r="C252" s="2" t="s">
+      <c r="C252" s="10" t="s">
         <v>3390</v>
       </c>
       <c r="D252" s="2" t="s">
@@ -42555,7 +42575,7 @@
       <c r="B253" s="2" t="s">
         <v>3393</v>
       </c>
-      <c r="C253" s="2" t="s">
+      <c r="C253" s="10" t="s">
         <v>3391</v>
       </c>
       <c r="D253" s="2" t="s">
@@ -42578,7 +42598,7 @@
       <c r="B254" s="2" t="s">
         <v>3393</v>
       </c>
-      <c r="C254" s="2" t="s">
+      <c r="C254" s="10" t="s">
         <v>3392</v>
       </c>
       <c r="D254" s="2" t="s">
@@ -42601,7 +42621,7 @@
       <c r="B255" s="2" t="s">
         <v>3394</v>
       </c>
-      <c r="C255" s="2" t="s">
+      <c r="C255" s="10" t="s">
         <v>3397</v>
       </c>
       <c r="D255" s="2" t="s">
@@ -42624,7 +42644,7 @@
       <c r="B256" s="2" t="s">
         <v>3394</v>
       </c>
-      <c r="C256" s="2" t="s">
+      <c r="C256" s="10" t="s">
         <v>3398</v>
       </c>
       <c r="D256" s="2" t="s">
@@ -42647,7 +42667,7 @@
       <c r="B257" s="2" t="s">
         <v>3399</v>
       </c>
-      <c r="C257" s="2" t="s">
+      <c r="C257" s="10" t="s">
         <v>3400</v>
       </c>
       <c r="D257" s="2" t="s">
@@ -42670,7 +42690,7 @@
       <c r="B258" s="2" t="s">
         <v>3399</v>
       </c>
-      <c r="C258" s="2" t="s">
+      <c r="C258" s="10" t="s">
         <v>3401</v>
       </c>
       <c r="D258" s="2" t="s">
@@ -42693,7 +42713,7 @@
       <c r="B259" s="2" t="s">
         <v>1771</v>
       </c>
-      <c r="C259" s="2" t="s">
+      <c r="C259" s="10" t="s">
         <v>1772</v>
       </c>
       <c r="D259" s="2" t="s">
@@ -42716,7 +42736,7 @@
       <c r="B260" s="2" t="s">
         <v>1773</v>
       </c>
-      <c r="C260" s="2" t="s">
+      <c r="C260" s="10" t="s">
         <v>1774</v>
       </c>
       <c r="D260" s="2" t="s">
@@ -42739,7 +42759,7 @@
       <c r="B261" s="2" t="s">
         <v>1773</v>
       </c>
-      <c r="C261" s="2" t="s">
+      <c r="C261" s="10" t="s">
         <v>1776</v>
       </c>
       <c r="D261" s="2" t="s">
@@ -42762,7 +42782,7 @@
       <c r="B262" s="2" t="s">
         <v>1773</v>
       </c>
-      <c r="C262" s="2" t="s">
+      <c r="C262" s="10" t="s">
         <v>1775</v>
       </c>
       <c r="D262" s="2" t="s">
@@ -42785,7 +42805,7 @@
       <c r="B263" s="2" t="s">
         <v>1773</v>
       </c>
-      <c r="C263" s="2" t="s">
+      <c r="C263" s="10" t="s">
         <v>1777</v>
       </c>
       <c r="D263" s="2" t="s">
@@ -42808,7 +42828,7 @@
       <c r="B264" s="2" t="s">
         <v>1773</v>
       </c>
-      <c r="C264" s="2" t="s">
+      <c r="C264" s="10" t="s">
         <v>1778</v>
       </c>
       <c r="D264" s="2" t="s">
@@ -42831,7 +42851,7 @@
       <c r="B265" s="2" t="s">
         <v>1773</v>
       </c>
-      <c r="C265" s="2" t="s">
+      <c r="C265" s="10" t="s">
         <v>1779</v>
       </c>
       <c r="D265" s="2" t="s">
@@ -42854,7 +42874,7 @@
       <c r="B266" s="2" t="s">
         <v>1780</v>
       </c>
-      <c r="C266" s="2" t="s">
+      <c r="C266" s="10" t="s">
         <v>1781</v>
       </c>
       <c r="D266" s="2" t="s">
@@ -42877,7 +42897,7 @@
       <c r="B267" s="2" t="s">
         <v>1780</v>
       </c>
-      <c r="C267" s="2" t="s">
+      <c r="C267" s="10" t="s">
         <v>1782</v>
       </c>
       <c r="D267" s="2" t="s">
@@ -42900,7 +42920,7 @@
       <c r="B268" s="2" t="s">
         <v>1780</v>
       </c>
-      <c r="C268" s="2" t="s">
+      <c r="C268" s="10" t="s">
         <v>1783</v>
       </c>
       <c r="D268" s="2" t="s">
@@ -42923,7 +42943,7 @@
       <c r="B269" s="2" t="s">
         <v>1780</v>
       </c>
-      <c r="C269" s="2" t="s">
+      <c r="C269" s="10" t="s">
         <v>1784</v>
       </c>
       <c r="D269" s="2" t="s">
@@ -42946,7 +42966,7 @@
       <c r="B270" s="2" t="s">
         <v>1785</v>
       </c>
-      <c r="C270" s="2" t="s">
+      <c r="C270" s="10" t="s">
         <v>1786</v>
       </c>
       <c r="D270" s="2" t="s">
@@ -42969,7 +42989,7 @@
       <c r="B271" s="2" t="s">
         <v>1785</v>
       </c>
-      <c r="C271" s="2" t="s">
+      <c r="C271" s="10" t="s">
         <v>1787</v>
       </c>
       <c r="D271" s="2" t="s">
@@ -42992,7 +43012,7 @@
       <c r="B272" s="2" t="s">
         <v>1785</v>
       </c>
-      <c r="C272" s="2" t="s">
+      <c r="C272" s="10" t="s">
         <v>1788</v>
       </c>
       <c r="D272" s="2" t="s">
@@ -43015,7 +43035,7 @@
       <c r="B273" s="2" t="s">
         <v>1785</v>
       </c>
-      <c r="C273" s="2" t="s">
+      <c r="C273" s="10" t="s">
         <v>1789</v>
       </c>
       <c r="D273" s="2" t="s">
@@ -43038,7 +43058,7 @@
       <c r="B274" s="2" t="s">
         <v>1785</v>
       </c>
-      <c r="C274" s="2" t="s">
+      <c r="C274" s="10" t="s">
         <v>1790</v>
       </c>
       <c r="D274" s="2" t="s">
@@ -43061,7 +43081,7 @@
       <c r="B275" s="2" t="s">
         <v>1785</v>
       </c>
-      <c r="C275" s="2" t="s">
+      <c r="C275" s="10" t="s">
         <v>1791</v>
       </c>
       <c r="D275" s="2" t="s">
@@ -43084,7 +43104,7 @@
       <c r="B276" s="2" t="s">
         <v>1785</v>
       </c>
-      <c r="C276" s="2" t="s">
+      <c r="C276" s="10" t="s">
         <v>1792</v>
       </c>
       <c r="D276" s="2" t="s">
@@ -43107,7 +43127,7 @@
       <c r="B277" s="2" t="s">
         <v>3402</v>
       </c>
-      <c r="C277" s="2" t="s">
+      <c r="C277" s="10" t="s">
         <v>3403</v>
       </c>
       <c r="D277" s="2" t="s">
@@ -43130,7 +43150,7 @@
       <c r="B278" s="2" t="s">
         <v>3402</v>
       </c>
-      <c r="C278" s="2" t="s">
+      <c r="C278" s="10" t="s">
         <v>3404</v>
       </c>
       <c r="D278" s="2" t="s">
@@ -43153,7 +43173,7 @@
       <c r="B279" s="2" t="s">
         <v>3402</v>
       </c>
-      <c r="C279" s="2" t="s">
+      <c r="C279" s="10" t="s">
         <v>3405</v>
       </c>
       <c r="D279" s="2" t="s">
@@ -43176,7 +43196,7 @@
       <c r="B280" s="2" t="s">
         <v>3402</v>
       </c>
-      <c r="C280" s="2" t="s">
+      <c r="C280" s="10" t="s">
         <v>3406</v>
       </c>
       <c r="D280" s="2" t="s">
@@ -43199,7 +43219,7 @@
       <c r="B281" s="2" t="s">
         <v>3402</v>
       </c>
-      <c r="C281" s="2" t="s">
+      <c r="C281" s="10" t="s">
         <v>3407</v>
       </c>
       <c r="D281" s="2" t="s">
@@ -43222,7 +43242,7 @@
       <c r="B282" s="2" t="s">
         <v>3402</v>
       </c>
-      <c r="C282" s="2" t="s">
+      <c r="C282" s="10" t="s">
         <v>3408</v>
       </c>
       <c r="D282" s="2" t="s">
@@ -43245,7 +43265,7 @@
       <c r="B283" s="2" t="s">
         <v>3402</v>
       </c>
-      <c r="C283" s="2" t="s">
+      <c r="C283" s="10" t="s">
         <v>3409</v>
       </c>
       <c r="D283" s="2" t="s">
@@ -43268,7 +43288,7 @@
       <c r="B284" s="2" t="s">
         <v>3402</v>
       </c>
-      <c r="C284" s="2" t="s">
+      <c r="C284" s="10" t="s">
         <v>3410</v>
       </c>
       <c r="D284" s="2" t="s">
@@ -43291,7 +43311,7 @@
       <c r="B285" s="2" t="s">
         <v>1085</v>
       </c>
-      <c r="C285" s="2"/>
+      <c r="C285" s="10"/>
       <c r="D285" s="2" t="s">
         <v>1085</v>
       </c>
@@ -43310,7 +43330,7 @@
       <c r="B286" s="2" t="s">
         <v>1086</v>
       </c>
-      <c r="C286" s="2"/>
+      <c r="C286" s="10"/>
       <c r="D286" s="2" t="s">
         <v>1086</v>
       </c>
@@ -43329,7 +43349,7 @@
       <c r="B287" s="2" t="s">
         <v>1087</v>
       </c>
-      <c r="C287" s="2"/>
+      <c r="C287" s="10"/>
       <c r="D287" s="2" t="s">
         <v>1087</v>
       </c>
@@ -43348,7 +43368,7 @@
       <c r="B288" s="2" t="s">
         <v>1088</v>
       </c>
-      <c r="C288" s="2"/>
+      <c r="C288" s="10"/>
       <c r="D288" s="2" t="s">
         <v>1088</v>
       </c>
@@ -43367,7 +43387,7 @@
       <c r="B289" s="2" t="s">
         <v>1667</v>
       </c>
-      <c r="C289" s="2" t="s">
+      <c r="C289" s="10" t="s">
         <v>1666</v>
       </c>
       <c r="D289" s="2" t="s">
@@ -43390,7 +43410,7 @@
       <c r="B290" s="2" t="s">
         <v>1794</v>
       </c>
-      <c r="C290" s="2" t="s">
+      <c r="C290" s="10" t="s">
         <v>1793</v>
       </c>
       <c r="D290" s="2" t="s">
@@ -43411,7 +43431,7 @@
       <c r="B291" s="2" t="s">
         <v>1091</v>
       </c>
-      <c r="C291" s="2" t="s">
+      <c r="C291" s="10" t="s">
         <v>1795</v>
       </c>
       <c r="D291" s="2" t="s">
@@ -43432,7 +43452,7 @@
         <v>439</v>
       </c>
       <c r="B292" s="2"/>
-      <c r="C292" s="2"/>
+      <c r="C292" s="10"/>
       <c r="D292" s="2" t="s">
         <v>3094</v>
       </c>
@@ -43449,7 +43469,7 @@
         <v>440</v>
       </c>
       <c r="B293" s="2"/>
-      <c r="C293" s="2"/>
+      <c r="C293" s="10"/>
       <c r="D293" s="2" t="s">
         <v>3095</v>
       </c>
@@ -43466,7 +43486,7 @@
         <v>441</v>
       </c>
       <c r="B294" s="2"/>
-      <c r="C294" s="2"/>
+      <c r="C294" s="10"/>
       <c r="D294" s="2" t="s">
         <v>3096</v>
       </c>
@@ -43483,7 +43503,7 @@
         <v>442</v>
       </c>
       <c r="B295" s="2"/>
-      <c r="C295" s="2"/>
+      <c r="C295" s="10"/>
       <c r="D295" s="2" t="s">
         <v>3097</v>
       </c>
@@ -43500,7 +43520,7 @@
         <v>443</v>
       </c>
       <c r="B296" s="2"/>
-      <c r="C296" s="2"/>
+      <c r="C296" s="10"/>
       <c r="D296" s="2" t="s">
         <v>3098</v>
       </c>
@@ -43517,7 +43537,7 @@
         <v>444</v>
       </c>
       <c r="B297" s="2"/>
-      <c r="C297" s="2"/>
+      <c r="C297" s="10"/>
       <c r="D297" s="2" t="s">
         <v>3099</v>
       </c>
@@ -43536,7 +43556,7 @@
       <c r="B298" s="2" t="s">
         <v>2042</v>
       </c>
-      <c r="C298" s="2" t="s">
+      <c r="C298" s="10" t="s">
         <v>1815</v>
       </c>
       <c r="D298" s="2" t="s">
@@ -43557,7 +43577,7 @@
       <c r="B299" s="2" t="s">
         <v>2042</v>
       </c>
-      <c r="C299" s="2" t="s">
+      <c r="C299" s="10" t="s">
         <v>1816</v>
       </c>
       <c r="D299" s="2" t="s">
@@ -43580,7 +43600,7 @@
       <c r="B300" s="2" t="s">
         <v>2033</v>
       </c>
-      <c r="C300" s="2" t="s">
+      <c r="C300" s="10" t="s">
         <v>1799</v>
       </c>
       <c r="D300" s="2" t="s">
@@ -43601,7 +43621,7 @@
       <c r="B301" s="2" t="s">
         <v>2033</v>
       </c>
-      <c r="C301" s="2" t="s">
+      <c r="C301" s="10" t="s">
         <v>1800</v>
       </c>
       <c r="D301" s="2" t="s">
@@ -43624,7 +43644,7 @@
       <c r="B302" s="2" t="s">
         <v>2036</v>
       </c>
-      <c r="C302" s="2" t="s">
+      <c r="C302" s="10" t="s">
         <v>1801</v>
       </c>
       <c r="D302" s="2" t="s">
@@ -43645,7 +43665,7 @@
       <c r="B303" s="2" t="s">
         <v>2036</v>
       </c>
-      <c r="C303" s="2" t="s">
+      <c r="C303" s="10" t="s">
         <v>1802</v>
       </c>
       <c r="D303" s="2" t="s">
@@ -43668,7 +43688,7 @@
       <c r="B304" s="2" t="s">
         <v>2037</v>
       </c>
-      <c r="C304" s="2" t="s">
+      <c r="C304" s="10" t="s">
         <v>1803</v>
       </c>
       <c r="D304" s="2" t="s">
@@ -43689,7 +43709,7 @@
       <c r="B305" s="2" t="s">
         <v>2037</v>
       </c>
-      <c r="C305" s="2" t="s">
+      <c r="C305" s="10" t="s">
         <v>1804</v>
       </c>
       <c r="D305" s="2" t="s">
@@ -43712,7 +43732,7 @@
       <c r="B306" s="2" t="s">
         <v>2038</v>
       </c>
-      <c r="C306" s="2" t="s">
+      <c r="C306" s="10" t="s">
         <v>1807</v>
       </c>
       <c r="D306" s="2" t="s">
@@ -43733,7 +43753,7 @@
       <c r="B307" s="2" t="s">
         <v>2038</v>
       </c>
-      <c r="C307" s="2" t="s">
+      <c r="C307" s="10" t="s">
         <v>1808</v>
       </c>
       <c r="D307" s="2" t="s">
@@ -43756,7 +43776,7 @@
       <c r="B308" s="2" t="s">
         <v>2034</v>
       </c>
-      <c r="C308" s="2" t="s">
+      <c r="C308" s="10" t="s">
         <v>1797</v>
       </c>
       <c r="D308" s="2" t="s">
@@ -43777,7 +43797,7 @@
       <c r="B309" s="2" t="s">
         <v>2034</v>
       </c>
-      <c r="C309" s="2" t="s">
+      <c r="C309" s="10" t="s">
         <v>1798</v>
       </c>
       <c r="D309" s="2" t="s">
@@ -43800,7 +43820,7 @@
       <c r="B310" s="2" t="s">
         <v>2039</v>
       </c>
-      <c r="C310" s="2" t="s">
+      <c r="C310" s="10" t="s">
         <v>1809</v>
       </c>
       <c r="D310" s="2" t="s">
@@ -43821,7 +43841,7 @@
       <c r="B311" s="2" t="s">
         <v>2039</v>
       </c>
-      <c r="C311" s="2" t="s">
+      <c r="C311" s="10" t="s">
         <v>1810</v>
       </c>
       <c r="D311" s="2" t="s">
@@ -43844,7 +43864,7 @@
       <c r="B312" s="2" t="s">
         <v>3413</v>
       </c>
-      <c r="C312" s="2" t="s">
+      <c r="C312" s="10" t="s">
         <v>3414</v>
       </c>
       <c r="D312" s="2" t="s">
@@ -43865,7 +43885,7 @@
       <c r="B313" s="2" t="s">
         <v>3413</v>
       </c>
-      <c r="C313" s="2" t="s">
+      <c r="C313" s="10" t="s">
         <v>3415</v>
       </c>
       <c r="D313" s="2" t="s">
@@ -43888,7 +43908,7 @@
       <c r="B314" s="2" t="s">
         <v>2040</v>
       </c>
-      <c r="C314" s="2" t="s">
+      <c r="C314" s="10" t="s">
         <v>1811</v>
       </c>
       <c r="D314" s="2" t="s">
@@ -43909,7 +43929,7 @@
       <c r="B315" s="2" t="s">
         <v>2040</v>
       </c>
-      <c r="C315" s="2" t="s">
+      <c r="C315" s="10" t="s">
         <v>1812</v>
       </c>
       <c r="D315" s="2" t="s">
@@ -43932,7 +43952,7 @@
       <c r="B316" s="2" t="s">
         <v>2038</v>
       </c>
-      <c r="C316" s="2" t="s">
+      <c r="C316" s="10" t="s">
         <v>1807</v>
       </c>
       <c r="D316" s="2" t="s">
@@ -43953,7 +43973,7 @@
       <c r="B317" s="2" t="s">
         <v>2038</v>
       </c>
-      <c r="C317" s="2" t="s">
+      <c r="C317" s="10" t="s">
         <v>1808</v>
       </c>
       <c r="D317" s="2" t="s">
@@ -43976,7 +43996,7 @@
       <c r="B318" s="2" t="s">
         <v>2041</v>
       </c>
-      <c r="C318" s="2" t="s">
+      <c r="C318" s="10" t="s">
         <v>1813</v>
       </c>
       <c r="D318" s="2" t="s">
@@ -43997,7 +44017,7 @@
       <c r="B319" s="2" t="s">
         <v>2041</v>
       </c>
-      <c r="C319" s="2" t="s">
+      <c r="C319" s="10" t="s">
         <v>1814</v>
       </c>
       <c r="D319" s="2" t="s">
@@ -44020,7 +44040,7 @@
       <c r="B320" s="2" t="s">
         <v>3419</v>
       </c>
-      <c r="C320" s="2" t="s">
+      <c r="C320" s="10" t="s">
         <v>3416</v>
       </c>
       <c r="D320" s="2" t="s">
@@ -44041,7 +44061,7 @@
       <c r="B321" s="2" t="s">
         <v>3419</v>
       </c>
-      <c r="C321" s="2" t="s">
+      <c r="C321" s="10" t="s">
         <v>3417</v>
       </c>
       <c r="D321" s="2" t="s">
@@ -44064,7 +44084,7 @@
       <c r="B322" s="2" t="s">
         <v>3420</v>
       </c>
-      <c r="C322" s="2" t="s">
+      <c r="C322" s="10" t="s">
         <v>3421</v>
       </c>
       <c r="D322" s="2" t="s">
@@ -44085,7 +44105,7 @@
       <c r="B323" s="2" t="s">
         <v>3420</v>
       </c>
-      <c r="C323" s="2" t="s">
+      <c r="C323" s="10" t="s">
         <v>3422</v>
       </c>
       <c r="D323" s="2" t="s">
@@ -44108,7 +44128,7 @@
       <c r="B324" s="2" t="s">
         <v>3423</v>
       </c>
-      <c r="C324" s="2" t="s">
+      <c r="C324" s="10" t="s">
         <v>3424</v>
       </c>
       <c r="D324" s="2" t="s">
@@ -44129,7 +44149,7 @@
       <c r="B325" s="2" t="s">
         <v>3423</v>
       </c>
-      <c r="C325" s="2" t="s">
+      <c r="C325" s="10" t="s">
         <v>3425</v>
       </c>
       <c r="D325" s="2" t="s">
@@ -44152,7 +44172,7 @@
       <c r="B326" s="2" t="s">
         <v>3426</v>
       </c>
-      <c r="C326" s="2" t="s">
+      <c r="C326" s="10" t="s">
         <v>3418</v>
       </c>
       <c r="D326" s="2" t="s">
@@ -44173,7 +44193,7 @@
       <c r="B327" s="2" t="s">
         <v>3426</v>
       </c>
-      <c r="C327" s="2" t="s">
+      <c r="C327" s="10" t="s">
         <v>3427</v>
       </c>
       <c r="D327" s="2" t="s">
@@ -44196,7 +44216,7 @@
       <c r="B328" s="2" t="s">
         <v>3428</v>
       </c>
-      <c r="C328" s="2" t="s">
+      <c r="C328" s="10" t="s">
         <v>3431</v>
       </c>
       <c r="D328" s="2" t="s">
@@ -44217,7 +44237,7 @@
       <c r="B329" s="2" t="s">
         <v>3428</v>
       </c>
-      <c r="C329" s="2" t="s">
+      <c r="C329" s="10" t="s">
         <v>3434</v>
       </c>
       <c r="D329" s="2" t="s">
@@ -44240,7 +44260,7 @@
       <c r="B330" s="2" t="s">
         <v>3429</v>
       </c>
-      <c r="C330" s="2" t="s">
+      <c r="C330" s="10" t="s">
         <v>3435</v>
       </c>
       <c r="D330" s="2" t="s">
@@ -44261,7 +44281,7 @@
       <c r="B331" s="2" t="s">
         <v>3429</v>
       </c>
-      <c r="C331" s="2" t="s">
+      <c r="C331" s="10" t="s">
         <v>3436</v>
       </c>
       <c r="D331" s="2" t="s">
@@ -44284,7 +44304,7 @@
       <c r="B332" s="2" t="s">
         <v>3430</v>
       </c>
-      <c r="C332" s="2" t="s">
+      <c r="C332" s="10" t="s">
         <v>3437</v>
       </c>
       <c r="D332" s="2" t="s">
@@ -44305,7 +44325,7 @@
       <c r="B333" s="2" t="s">
         <v>3430</v>
       </c>
-      <c r="C333" s="2" t="s">
+      <c r="C333" s="10" t="s">
         <v>3438</v>
       </c>
       <c r="D333" s="2" t="s">
@@ -44328,7 +44348,7 @@
       <c r="B334" s="2" t="s">
         <v>3439</v>
       </c>
-      <c r="C334" s="2" t="s">
+      <c r="C334" s="10" t="s">
         <v>3432</v>
       </c>
       <c r="D334" s="2" t="s">
@@ -44349,7 +44369,7 @@
       <c r="B335" s="2" t="s">
         <v>3439</v>
       </c>
-      <c r="C335" s="2" t="s">
+      <c r="C335" s="10" t="s">
         <v>3433</v>
       </c>
       <c r="D335" s="2" t="s">
@@ -44372,7 +44392,7 @@
       <c r="B336" s="2" t="s">
         <v>3440</v>
       </c>
-      <c r="C336" s="2" t="s">
+      <c r="C336" s="10" t="s">
         <v>3443</v>
       </c>
       <c r="D336" s="2" t="s">
@@ -44393,7 +44413,7 @@
       <c r="B337" s="2" t="s">
         <v>3440</v>
       </c>
-      <c r="C337" s="2" t="s">
+      <c r="C337" s="10" t="s">
         <v>3444</v>
       </c>
       <c r="D337" s="2" t="s">
@@ -44416,7 +44436,7 @@
       <c r="B338" s="2" t="s">
         <v>3441</v>
       </c>
-      <c r="C338" s="2" t="s">
+      <c r="C338" s="10" t="s">
         <v>3445</v>
       </c>
       <c r="D338" s="2" t="s">
@@ -44437,7 +44457,7 @@
       <c r="B339" s="2" t="s">
         <v>3441</v>
       </c>
-      <c r="C339" s="2" t="s">
+      <c r="C339" s="10" t="s">
         <v>3446</v>
       </c>
       <c r="D339" s="2" t="s">
@@ -44460,7 +44480,7 @@
       <c r="B340" s="2" t="s">
         <v>3447</v>
       </c>
-      <c r="C340" s="2" t="s">
+      <c r="C340" s="10" t="s">
         <v>3450</v>
       </c>
       <c r="D340" s="2" t="s">
@@ -44481,7 +44501,7 @@
       <c r="B341" s="2" t="s">
         <v>3447</v>
       </c>
-      <c r="C341" s="2" t="s">
+      <c r="C341" s="10" t="s">
         <v>3442</v>
       </c>
       <c r="D341" s="2" t="s">
@@ -44504,7 +44524,7 @@
       <c r="B342" s="2" t="s">
         <v>3448</v>
       </c>
-      <c r="C342" s="2" t="s">
+      <c r="C342" s="10" t="s">
         <v>3451</v>
       </c>
       <c r="D342" s="2" t="s">
@@ -44525,7 +44545,7 @@
       <c r="B343" s="2" t="s">
         <v>3448</v>
       </c>
-      <c r="C343" s="2" t="s">
+      <c r="C343" s="10" t="s">
         <v>3452</v>
       </c>
       <c r="D343" s="2" t="s">
@@ -44548,7 +44568,7 @@
       <c r="B344" s="2" t="s">
         <v>3449</v>
       </c>
-      <c r="C344" s="2" t="s">
+      <c r="C344" s="10" t="s">
         <v>3453</v>
       </c>
       <c r="D344" s="2" t="s">
@@ -44569,7 +44589,7 @@
       <c r="B345" s="2" t="s">
         <v>3449</v>
       </c>
-      <c r="C345" s="2" t="s">
+      <c r="C345" s="10" t="s">
         <v>3454</v>
       </c>
       <c r="D345" s="2" t="s">
@@ -44592,7 +44612,7 @@
       <c r="B346" s="2" t="s">
         <v>2043</v>
       </c>
-      <c r="C346" s="2" t="s">
+      <c r="C346" s="10" t="s">
         <v>1818</v>
       </c>
       <c r="D346" s="2" t="s">
@@ -44613,7 +44633,7 @@
       <c r="B347" s="2" t="s">
         <v>2043</v>
       </c>
-      <c r="C347" s="2" t="s">
+      <c r="C347" s="10" t="s">
         <v>1817</v>
       </c>
       <c r="D347" s="2" t="s">
@@ -44636,7 +44656,7 @@
       <c r="B348" s="2" t="s">
         <v>1120</v>
       </c>
-      <c r="C348" s="2" t="s">
+      <c r="C348" s="10" t="s">
         <v>1819</v>
       </c>
       <c r="D348" s="2" t="s">
@@ -44657,7 +44677,7 @@
       <c r="B349" s="2" t="s">
         <v>1915</v>
       </c>
-      <c r="C349" s="2" t="s">
+      <c r="C349" s="10" t="s">
         <v>1939</v>
       </c>
       <c r="D349" s="2" t="s">
@@ -44680,7 +44700,7 @@
       <c r="B350" s="2" t="s">
         <v>1121</v>
       </c>
-      <c r="C350" s="2" t="s">
+      <c r="C350" s="10" t="s">
         <v>1820</v>
       </c>
       <c r="D350" s="2" t="s">
@@ -44703,7 +44723,7 @@
       <c r="B351" s="2" t="s">
         <v>1122</v>
       </c>
-      <c r="C351" s="2" t="s">
+      <c r="C351" s="10" t="s">
         <v>1821</v>
       </c>
       <c r="D351" s="2" t="s">

</xml_diff>